<commit_message>
starting on permanent attributes...
</commit_message>
<xml_diff>
--- a/plans/todo.xlsx
+++ b/plans/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edsquid\Documents\Personal Projects\Business\RogueLikeGame\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1D7F5E-B9C1-4706-AA7D-9BE31AB012D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC1159C-A320-4922-8CF4-35319D865F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="7170" windowHeight="15585" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="3" r:id="rId1"/>
@@ -297,9 +297,6 @@
     <t>Damage type increase</t>
   </si>
   <si>
-    <t xml:space="preserve">Damage Type Resistence </t>
-  </si>
-  <si>
     <t>Attributes Detailed</t>
   </si>
   <si>
@@ -715,6 +712,9 @@
   </si>
   <si>
     <t xml:space="preserve">remove second weapon, add dual wield </t>
+  </si>
+  <si>
+    <t>Damage Type Resistence (all types)</t>
   </si>
 </sst>
 </file>
@@ -975,6 +975,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -999,6 +1000,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1006,6 +1013,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1017,19 +1030,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1347,7 +1347,7 @@
   <dimension ref="A1:H338"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,79 +1364,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="A1" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="G3" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="A4" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" s="3">
         <v>0.05</v>
@@ -1448,16 +1448,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E6" s="3">
         <v>0.05</v>
@@ -1472,13 +1472,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E7" s="3">
         <v>0.05</v>
@@ -1493,13 +1493,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E8" s="3">
         <v>0.05</v>
@@ -1514,13 +1514,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" s="3">
         <v>0.05</v>
@@ -1535,13 +1535,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E10" s="3">
         <v>0.05</v>
@@ -1556,13 +1556,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E11" s="3">
         <v>0.05</v>
@@ -1577,13 +1577,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E12" s="3">
         <v>0.05</v>
@@ -1598,13 +1598,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E13" s="3">
         <v>0.05</v>
@@ -1619,13 +1619,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E14" s="3">
         <v>0.05</v>
@@ -1640,13 +1640,13 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E15" s="3">
         <v>0.05</v>
@@ -1661,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E16" s="3">
         <v>0.05</v>
@@ -1682,13 +1682,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E17" s="3">
         <v>0.05</v>
@@ -1703,13 +1703,13 @@
         <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E18" s="3">
         <v>0.05</v>
@@ -1724,13 +1724,13 @@
         <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E19" s="3">
         <v>0.05</v>
@@ -1742,16 +1742,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20" s="3">
         <v>0.05</v>
@@ -1763,16 +1763,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E21" s="3">
         <v>0.05</v>
@@ -1784,16 +1784,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E22" s="3">
         <v>0.01</v>
@@ -1808,13 +1808,13 @@
         <v>83</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E23" s="3">
         <v>0.05</v>
@@ -1829,13 +1829,13 @@
         <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E24" s="3">
         <v>0.05</v>
@@ -1846,17 +1846,17 @@
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
-        <v>86</v>
+      <c r="A25" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E25" s="3">
         <v>0.05</v>
@@ -1871,13 +1871,13 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -1907,48 +1907,48 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F35" s="1">
         <v>10</v>
@@ -1957,16 +1957,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F36" s="1">
         <v>10</v>
@@ -1978,13 +1978,13 @@
         <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F37" s="1">
         <v>10</v>
@@ -1996,13 +1996,13 @@
         <v>16</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
@@ -2014,13 +2014,13 @@
         <v>17</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F39" s="1">
         <v>5</v>
@@ -2038,48 +2038,48 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="D43" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
+      <c r="A44" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="F45" s="1">
         <v>5</v>
@@ -2088,16 +2088,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F46" s="1">
         <v>5</v>
@@ -2106,16 +2106,16 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F47" s="1">
         <v>5</v>
@@ -2136,13 +2136,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F50" s="1">
         <v>5</v>
@@ -2151,13 +2151,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F51" s="1">
         <v>5</v>
@@ -2166,13 +2166,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="F52" s="1">
         <v>5</v>
@@ -2181,16 +2181,16 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C53" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="F53" s="1">
         <v>5</v>
@@ -2205,13 +2205,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F55" s="1">
         <v>5</v>
@@ -2238,13 +2238,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F59" s="1">
         <v>5</v>
@@ -2253,13 +2253,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F60" s="1">
         <v>5</v>
@@ -2268,13 +2268,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F61" s="1">
         <v>5</v>
@@ -2283,13 +2283,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="F62" s="1">
         <v>5</v>
@@ -2298,10 +2298,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F63" s="1">
         <v>5</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F65" s="1">
         <v>5</v>
@@ -2331,10 +2331,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F66" s="1">
         <v>5</v>
@@ -2343,13 +2343,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F67" s="1">
         <v>5</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F68" s="1">
         <v>5</v>
@@ -2373,13 +2373,13 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F69" s="1">
         <v>5</v>
@@ -2388,7 +2388,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G70" s="3"/>
     </row>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F73" s="1">
         <v>5</v>
@@ -2412,10 +2412,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F74" s="1">
         <v>5</v>
@@ -2424,10 +2424,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F75" s="1">
         <v>5</v>
@@ -2448,10 +2448,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F78" s="1">
         <v>5</v>
@@ -2472,10 +2472,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F81" s="1">
         <v>5</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F82" s="1">
         <v>5</v>
@@ -2496,10 +2496,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F83" s="1">
         <v>5</v>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F85" s="1">
         <v>5</v>
@@ -2526,10 +2526,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F86" s="1">
         <v>5</v>
@@ -2538,10 +2538,10 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F87" s="1">
         <v>5</v>
@@ -2562,10 +2562,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F90" s="1">
         <v>5</v>
@@ -2574,10 +2574,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F91" s="1">
         <v>5</v>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F93" s="1">
         <v>5</v>
@@ -2607,10 +2607,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F95" s="1">
         <v>5</v>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F97" s="1">
         <v>5</v>
@@ -2640,7 +2640,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F99" s="1">
         <v>5</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F100" s="1">
         <v>5</v>
@@ -2658,7 +2658,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F101" s="1">
         <v>5</v>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F102" s="1">
         <v>5</v>
@@ -2694,7 +2694,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F106" s="1">
         <v>5</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F107" s="1">
         <v>5</v>
@@ -2724,7 +2724,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F110" s="1">
         <v>5</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F112" s="1">
         <v>5</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F116" s="1">
         <v>5</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F117" s="1">
         <v>5</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F118" s="1">
         <v>5</v>
@@ -2796,7 +2796,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F119" s="1">
         <v>5</v>
@@ -2805,7 +2805,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F120" s="1">
         <v>5</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F124" s="1">
         <v>5</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F125" s="1">
         <v>5</v>
@@ -2859,7 +2859,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F127" s="1">
         <v>5</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F128" s="1">
         <v>5</v>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F129" s="1">
         <v>5</v>
@@ -2904,39 +2904,39 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B133" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B133" s="5" t="s">
+      <c r="C133" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C133" s="5" t="s">
+      <c r="D133" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F133" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D133" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E133" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F133" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="G133" s="5"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="B134" s="15"/>
-      <c r="C134" s="15"/>
-      <c r="D134" s="15"/>
-      <c r="E134" s="15"/>
-      <c r="F134" s="15"/>
-      <c r="G134" s="15"/>
+      <c r="A134" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B134" s="16"/>
+      <c r="C134" s="16"/>
+      <c r="D134" s="16"/>
+      <c r="E134" s="16"/>
+      <c r="F134" s="16"/>
+      <c r="G134" s="16"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F135" s="1">
         <v>1</v>
@@ -2981,7 +2981,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F140" s="1">
         <v>1</v>
@@ -3017,7 +3017,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F144" s="1">
         <v>1</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F145" s="1">
         <v>1</v>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F153" s="1">
         <v>1</v>
@@ -4249,309 +4249,309 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25" t="s">
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+    </row>
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="31"/>
+      <c r="J3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AA3" s="32"/>
+      <c r="AB3" s="32"/>
+    </row>
+    <row r="4" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-    </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="W3" s="26"/>
-      <c r="X3" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="27"/>
-    </row>
-    <row r="4" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="24" t="s">
+      <c r="P4" s="27"/>
+      <c r="Q4" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="23" t="s">
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="W4" s="27"/>
+      <c r="X4" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+    </row>
+    <row r="5" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="J5" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="W4" s="24"/>
-      <c r="X4" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-    </row>
-    <row r="5" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="24" t="s">
+      <c r="P5" s="27"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="W5" s="27"/>
+      <c r="X5" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+    </row>
+    <row r="6" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="25"/>
+      <c r="J6" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="W5" s="24"/>
-      <c r="X5" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="23"/>
-    </row>
-    <row r="6" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="24" t="s">
+      <c r="P6" s="27"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="W6" s="27"/>
+      <c r="X6" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+    </row>
+    <row r="7" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="25"/>
+      <c r="J7" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="W6" s="24"/>
-      <c r="X6" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-    </row>
-    <row r="7" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="24" t="s">
+      <c r="P7" s="27"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="W7" s="24"/>
-      <c r="X7" s="23" t="s">
+      <c r="W7" s="27"/>
+      <c r="X7" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
     </row>
     <row r="8" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="28" t="s">
         <v>55</v>
       </c>
@@ -4563,977 +4563,761 @@
       <c r="L8" s="29"/>
       <c r="M8" s="29"/>
       <c r="N8" s="29"/>
-      <c r="O8" s="24" t="s">
+      <c r="O8" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="24" t="s">
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="26"/>
+      <c r="V8" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="W8" s="24"/>
-      <c r="X8" s="23" t="s">
+      <c r="W8" s="27"/>
+      <c r="X8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="26"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
     </row>
     <row r="9" spans="1:28" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="22" t="s">
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23" t="s">
+      <c r="I9" s="25"/>
+      <c r="J9" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="24" t="s">
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="W9" s="24"/>
-      <c r="X9" s="23" t="s">
+      <c r="W9" s="27"/>
+      <c r="X9" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
     </row>
     <row r="10" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="22" t="s">
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="23" t="s">
+      <c r="I10" s="25"/>
+      <c r="J10" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="24" t="s">
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="W10" s="24"/>
-      <c r="X10" s="23" t="s">
+      <c r="W10" s="27"/>
+      <c r="X10" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="Y10" s="23"/>
-      <c r="Z10" s="23"/>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="23"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="26"/>
+      <c r="AA10" s="26"/>
+      <c r="AB10" s="26"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="22" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23" t="s">
+      <c r="I11" s="25"/>
+      <c r="J11" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="24" t="s">
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="W11" s="24"/>
-      <c r="X11" s="23" t="s">
+      <c r="W11" s="27"/>
+      <c r="X11" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="26"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="22" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="26"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="24"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="26"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="23"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="23"/>
-      <c r="AB14" s="23"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="26"/>
+      <c r="AB14" s="26"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="26"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="26"/>
+      <c r="Y16" s="26"/>
+      <c r="Z16" s="26"/>
+      <c r="AA16" s="26"/>
+      <c r="AB16" s="26"/>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="23"/>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="26"/>
+      <c r="AA17" s="26"/>
+      <c r="AB17" s="26"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="23"/>
-      <c r="Z18" s="23"/>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="23"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="26"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="26"/>
+      <c r="Y18" s="26"/>
+      <c r="Z18" s="26"/>
+      <c r="AA18" s="26"/>
+      <c r="AB18" s="26"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="23"/>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="26"/>
+      <c r="Z19" s="26"/>
+      <c r="AA19" s="26"/>
+      <c r="AB19" s="26"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="23"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="23"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="26"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="23"/>
-      <c r="Z21" s="23"/>
-      <c r="AA21" s="23"/>
-      <c r="AB21" s="23"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="26"/>
+      <c r="Y21" s="26"/>
+      <c r="Z21" s="26"/>
+      <c r="AA21" s="26"/>
+      <c r="AB21" s="26"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="23"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="23"/>
-      <c r="Y22" s="23"/>
-      <c r="Z22" s="23"/>
-      <c r="AA22" s="23"/>
-      <c r="AB22" s="23"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="26"/>
+      <c r="Z22" s="26"/>
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="26"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="23"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="23"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="26"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="23"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="26"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="26"/>
+      <c r="U27" s="26"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="23"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="26"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="26"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="26"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
-      <c r="Q33" s="23"/>
-      <c r="R33" s="23"/>
-      <c r="S33" s="23"/>
-      <c r="T33" s="23"/>
-      <c r="U33" s="23"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="31"/>
-      <c r="R34" s="31"/>
-      <c r="S34" s="31"/>
-      <c r="T34" s="31"/>
-      <c r="U34" s="31"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
+      <c r="T34" s="24"/>
+      <c r="U34" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="236">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:U34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:U33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:U32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:U31"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:U30"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:U29"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:U28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:U26"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:U25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:U24"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:U23"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="X22:AB22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:AB21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:U21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:U22"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="X20:AB20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="X19:AB19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:U19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:U20"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:AB18"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:AB17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:U17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:U18"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:N16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="X16:AB16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="X15:AB15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:U15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:U16"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="X14:AB14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="X13:AB13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q13:U13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:N12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="X12:AB12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="X11:AB11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:U11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:U12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:AB10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:U10"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:AB8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:AB7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:AB5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:U6"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="H4:I4"/>
@@ -5554,6 +5338,222 @@
     <mergeCell ref="Q3:U3"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:AB5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:AB7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:U10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:N12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="X12:AB12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="X11:AB11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:U11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:U12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="X14:AB14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="X13:AB13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q13:U13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:N16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="X16:AB16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="X15:AB15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:U16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="X18:AB18"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:AB17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:U17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:U18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="X20:AB20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="X19:AB19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:U19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:U20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="X22:AB22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:AB21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:U21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:U22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:U24"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:U23"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:U26"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:U28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:U30"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:U29"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:U32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:U31"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:U34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:U33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
found some resources, added some functionality
</commit_message>
<xml_diff>
--- a/plans/todo.xlsx
+++ b/plans/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edsquid\Documents\Personal Projects\Business\RogueLikeGame\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4C75BA-BB77-457A-8EAC-711E76E07FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9278C4-B7DF-40DF-87F8-3460AEBFB888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5400" yWindow="2880" windowWidth="21600" windowHeight="11295" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="338">
   <si>
     <t>Max Lives</t>
   </si>
@@ -1049,6 +1049,12 @@
   </si>
   <si>
     <t>Knockback</t>
+  </si>
+  <si>
+    <t>Shroom Runner</t>
+  </si>
+  <si>
+    <t>Yea yea</t>
   </si>
 </sst>
 </file>
@@ -1403,6 +1409,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1411,9 +1420,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1747,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CE061F-AFA4-4B9D-BFD1-A05915568E6D}">
   <dimension ref="A1:H338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4900,121 +4906,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35" t="s">
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35" t="s">
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
       <c r="AD1" s="19" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="36" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37" t="s">
+      <c r="I3" s="37"/>
+      <c r="J3" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="36" t="s">
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="37" t="s">
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="36" t="s">
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="W3" s="36"/>
-      <c r="X3" s="37" t="s">
+      <c r="W3" s="37"/>
+      <c r="X3" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
     </row>
     <row r="4" spans="1:30" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
@@ -5377,13 +5383,13 @@
         <v>269</v>
       </c>
       <c r="B12" s="32"/>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
       <c r="H12" s="32" t="s">
         <v>76</v>
       </c>
@@ -5415,13 +5421,13 @@
         <v>274</v>
       </c>
       <c r="B13" s="32"/>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
       <c r="H13" s="32" t="s">
         <v>46</v>
       </c>
@@ -5461,13 +5467,13 @@
         <v>278</v>
       </c>
       <c r="B14" s="32"/>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="35" t="s">
         <v>277</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="33"/>
@@ -5495,7 +5501,7 @@
         <v>279</v>
       </c>
       <c r="B15" s="32"/>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="35" t="s">
         <v>280</v>
       </c>
       <c r="D15" s="33"/>
@@ -6012,147 +6018,77 @@
     </row>
   </sheetData>
   <mergeCells count="236">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:U34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:U33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:U32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:U31"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:U30"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:U29"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:U28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:U26"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:U25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:U24"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:U23"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="X22:AB22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:AB21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:U21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:U22"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="X20:AB20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="X19:AB19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:U19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:U20"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:AB18"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:AB17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:U17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:U18"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="X16:AB16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="X15:AB15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:U15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:U16"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="X14:AB14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="X13:AB13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:AB4"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:N2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="V1:AB2"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="O1:U2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:AB5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:AB7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:U10"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="H16:I16"/>
@@ -6177,77 +6113,147 @@
     <mergeCell ref="Q13:U13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:G14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:AB10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:U10"/>
-    <mergeCell ref="X8:AB8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:AB7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:AB5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:AB4"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:N2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="V1:AB2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="O1:U2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="X14:AB14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="X13:AB13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="X16:AB16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="X15:AB15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:U16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="X18:AB18"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:AB17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:U17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:U18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="X20:AB20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="X19:AB19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:U19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:U20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="X22:AB22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:AB21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:U21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:U22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:U24"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:U23"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:U26"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:U28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:U30"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:U29"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:U32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:U31"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:U34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:U33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C15" r:id="rId1" xr:uid="{868F8F85-B252-4B04-B081-E9B23AD46A23}"/>
@@ -6264,8 +6270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1908B5E3-0D9D-48A8-894B-90B53E0249A0}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6492,7 +6498,21 @@
       <c r="H13" s="39"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="39"/>
+      <c r="A14" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="C14" s="21">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>337</v>
+      </c>
       <c r="F14" s="39"/>
       <c r="G14" s="39"/>
       <c r="H14" s="39"/>
@@ -6571,14 +6591,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="E8:H8"/>
@@ -6591,12 +6609,14 @@
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E24:H24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6881,6 +6901,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="D20:G20"/>
@@ -6893,23 +6930,6 @@
     <mergeCell ref="D27:G27"/>
     <mergeCell ref="D28:G28"/>
     <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished lame ah attributes
</commit_message>
<xml_diff>
--- a/plans/todo.xlsx
+++ b/plans/todo.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edsquid\Documents\Personal Projects\Business\RogueLikeGame\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90297A16-2F28-41CC-88F4-EEACC20D1CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C799F5-38A7-4EE5-9CC5-A6AC714F2703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29910" yWindow="1620" windowWidth="18900" windowHeight="13530" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
+    <workbookView xWindow="14985" yWindow="795" windowWidth="13470" windowHeight="13740" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
-    <sheet name="Maps" sheetId="5" r:id="rId3"/>
-    <sheet name="Characters" sheetId="4" r:id="rId4"/>
-    <sheet name="Weapons and Secondary" sheetId="2" r:id="rId5"/>
-    <sheet name="Enemies" sheetId="6" r:id="rId6"/>
-    <sheet name="Interactables" sheetId="7" r:id="rId7"/>
+    <sheet name="Maps" sheetId="5" r:id="rId2"/>
+    <sheet name="Characters" sheetId="4" r:id="rId3"/>
+    <sheet name="Weapons and Secondary" sheetId="2" r:id="rId4"/>
+    <sheet name="Enemies" sheetId="6" r:id="rId5"/>
+    <sheet name="Interactables" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="361">
   <si>
     <t>Max Lives</t>
   </si>
@@ -110,9 +109,6 @@
     <t xml:space="preserve">Each and every day (Increase health regen) </t>
   </si>
   <si>
-    <t>Increase max damage, reduce min damage (able to heal enemies)</t>
-  </si>
-  <si>
     <t>Crit chance</t>
   </si>
   <si>
@@ -131,9 +127,6 @@
     <t>Reduce max ammo, reduce reload time</t>
   </si>
   <si>
-    <t>Reduce regular damage, increase status effect potency</t>
-  </si>
-  <si>
     <t xml:space="preserve">Increase base damage 200%, add 10 lives, max health set to 1 </t>
   </si>
   <si>
@@ -560,9 +553,6 @@
     <t>Keys</t>
   </si>
   <si>
-    <t>Roll the dice champ. "+50% crit chance, +25% crit damage, -50% base damage"</t>
-  </si>
-  <si>
     <t>Remove stamina bar, stamina actions reduce health, increase health regen by 200%</t>
   </si>
   <si>
@@ -1115,25 +1105,25 @@
     <t>Seconds please (Increase size, increase health, reduce speed)</t>
   </si>
   <si>
-    <t>putYourWeightIntoIt (more health = more melee dmg)</t>
-  </si>
-  <si>
     <t>battleScars, Remove ability to dash, double base health</t>
   </si>
   <si>
-    <t>Types</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>ratio of total</t>
-  </si>
-  <si>
-    <t>w/ weight</t>
-  </si>
-  <si>
     <t>Explosive Dash - Fire, Frost</t>
+  </si>
+  <si>
+    <t>Chaotic Chances - Increase max damage, reduce min damage (able to heal enemies)</t>
+  </si>
+  <si>
+    <t>Balancing Technique - Opposite</t>
+  </si>
+  <si>
+    <t>putYourBackIntoIt (more health = more melee dmg)</t>
+  </si>
+  <si>
+    <t>potion sellar - Reduce regular damage, increase status effect potency</t>
+  </si>
+  <si>
+    <t>Roll the dice champ. "+25% crit chance, +25% crit damage, -50% base damage"</t>
   </si>
 </sst>
 </file>
@@ -1420,7 +1410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1495,9 +1485,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1506,6 +1493,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1522,7 +1512,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1840,8 +1829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CE061F-AFA4-4B9D-BFD1-A05915568E6D}">
   <dimension ref="A1:H338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,7 +1848,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -1868,7 +1857,7 @@
       <c r="F1" s="29"/>
       <c r="G1" s="29"/>
       <c r="H1" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1880,36 +1869,36 @@
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
       <c r="H2" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="G3" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -1921,16 +1910,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E5" s="2">
         <v>0.05</v>
@@ -1942,16 +1931,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6" s="2">
         <v>0.05</v>
@@ -1966,13 +1955,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E7" s="2">
         <v>0.05</v>
@@ -1987,13 +1976,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E8" s="2">
         <v>0.05</v>
@@ -2008,13 +1997,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E9" s="2">
         <v>0.05</v>
@@ -2029,13 +2018,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E10" s="2">
         <v>0.05</v>
@@ -2050,13 +2039,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E11" s="2">
         <v>0.05</v>
@@ -2071,13 +2060,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E12" s="2">
         <v>0.05</v>
@@ -2092,13 +2081,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E13" s="2">
         <v>0.05</v>
@@ -2113,13 +2102,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E14" s="2">
         <v>0.05</v>
@@ -2134,13 +2123,13 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E15" s="2">
         <v>0.05</v>
@@ -2155,13 +2144,13 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E16" s="2">
         <v>0.05</v>
@@ -2176,13 +2165,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E17" s="2">
         <v>0.05</v>
@@ -2194,16 +2183,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E18" s="2">
         <v>0.05</v>
@@ -2215,16 +2204,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E19" s="2">
         <v>0.05</v>
@@ -2236,16 +2225,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E20" s="2">
         <v>0.05</v>
@@ -2257,16 +2246,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E21" s="2">
         <v>0.05</v>
@@ -2278,16 +2267,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E22" s="2">
         <v>0.01</v>
@@ -2299,16 +2288,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E23" s="2">
         <v>0.05</v>
@@ -2320,16 +2309,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E24" s="2">
         <v>0.05</v>
@@ -2341,16 +2330,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E25" s="2">
         <v>0.05</v>
@@ -2365,13 +2354,13 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
@@ -2383,7 +2372,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G27" s="2"/>
     </row>
@@ -2404,22 +2393,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="D33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="G33" s="4"/>
     </row>
@@ -2436,16 +2425,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F35" s="1">
         <v>10</v>
@@ -2454,16 +2443,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="D36" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F36" s="1">
         <v>10</v>
@@ -2475,13 +2464,13 @@
         <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F37" s="1">
         <v>10</v>
@@ -2493,13 +2482,13 @@
         <v>16</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
@@ -2511,13 +2500,13 @@
         <v>17</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F39" s="1">
         <v>5</v>
@@ -2526,13 +2515,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F40" s="1">
         <v>10</v>
@@ -2547,28 +2536,28 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="D43" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
@@ -2579,16 +2568,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F45" s="1">
         <v>5</v>
@@ -2600,13 +2589,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F47" s="1">
         <v>5</v>
@@ -2615,16 +2604,16 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F48" s="1">
         <v>5</v>
@@ -2639,13 +2628,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="F50" s="1">
         <v>5</v>
@@ -2657,7 +2646,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F52" s="1">
         <v>5</v>
@@ -2666,13 +2655,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F54" s="1">
         <v>5</v>
@@ -2681,13 +2670,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="F55" s="1">
         <v>5</v>
@@ -2696,13 +2685,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F56" s="1">
         <v>5</v>
@@ -2711,7 +2700,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2722,10 +2711,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F59" s="1">
         <v>5</v>
@@ -2743,13 +2732,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F65" s="1">
         <v>5</v>
@@ -2758,10 +2747,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F66" s="1">
         <v>5</v>
@@ -2770,13 +2759,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F67" s="1">
         <v>5</v>
@@ -2785,13 +2774,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F68" s="1">
         <v>5</v>
@@ -2800,13 +2789,13 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F69" s="1">
         <v>5</v>
@@ -2815,7 +2804,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G70" s="2"/>
     </row>
@@ -2830,7 +2819,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F73" s="1">
         <v>5</v>
@@ -2839,10 +2828,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F74" s="1">
         <v>5</v>
@@ -2851,10 +2840,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F75" s="1">
         <v>5</v>
@@ -2875,10 +2864,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F78" s="1">
         <v>5</v>
@@ -2887,7 +2876,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F79" s="1">
         <v>5</v>
@@ -2902,10 +2891,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F81" s="1">
         <v>5</v>
@@ -2914,10 +2903,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F82" s="1">
         <v>5</v>
@@ -2935,10 +2924,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F85" s="1">
         <v>5</v>
@@ -2947,10 +2936,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F86" s="1">
         <v>5</v>
@@ -2959,10 +2948,10 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F87" s="1">
         <v>5</v>
@@ -2971,7 +2960,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F88" s="1">
         <v>5</v>
@@ -2986,10 +2975,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F90" s="1">
         <v>5</v>
@@ -2998,10 +2987,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F91" s="1">
         <v>5</v>
@@ -3010,10 +2999,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F92" s="1">
         <v>5</v>
@@ -3022,7 +3011,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F93" s="1">
         <v>5</v>
@@ -3031,10 +3020,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F95" s="1">
         <v>5</v>
@@ -3049,7 +3038,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F97" s="1">
         <v>5</v>
@@ -3064,7 +3053,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F99" s="1">
         <v>5</v>
@@ -3073,7 +3062,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F100" s="1">
         <v>5</v>
@@ -3082,7 +3071,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F101" s="1">
         <v>5</v>
@@ -3091,7 +3080,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F102" s="1">
         <v>5</v>
@@ -3118,7 +3107,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F106" s="1">
         <v>5</v>
@@ -3127,7 +3116,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F107" s="1">
         <v>5</v>
@@ -3148,7 +3137,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F110" s="1">
         <v>5</v>
@@ -3163,7 +3152,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F112" s="1">
         <v>5</v>
@@ -3184,7 +3173,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F116" s="1">
         <v>5</v>
@@ -3193,7 +3182,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F117" s="1">
         <v>5</v>
@@ -3202,7 +3191,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F118" s="1">
         <v>5</v>
@@ -3211,7 +3200,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F119" s="1">
         <v>5</v>
@@ -3220,7 +3209,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F120" s="1">
         <v>5</v>
@@ -3250,7 +3239,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F124" s="1">
         <v>5</v>
@@ -3259,7 +3248,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F125" s="1">
         <v>5</v>
@@ -3274,7 +3263,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F127" s="1">
         <v>5</v>
@@ -3283,7 +3272,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F128" s="1">
         <v>5</v>
@@ -3292,7 +3281,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F129" s="1">
         <v>5</v>
@@ -3319,28 +3308,28 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C133" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="D133" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F133" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D133" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E133" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F133" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="G133" s="4"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B134" s="25"/>
       <c r="C134" s="25"/>
@@ -3351,7 +3340,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F135" s="1">
         <v>1</v>
@@ -3387,7 +3376,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F139" s="1">
         <v>1</v>
@@ -3396,7 +3385,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F140" s="1">
         <v>1</v>
@@ -3414,7 +3403,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>22</v>
+        <v>356</v>
       </c>
       <c r="F142" s="1">
         <v>1</v>
@@ -3422,21 +3411,24 @@
       <c r="G142" s="2"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="F143" s="1">
         <v>1</v>
       </c>
       <c r="G143" s="2"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>357</v>
+      </c>
       <c r="F144" s="1">
         <v>1</v>
       </c>
       <c r="G144" s="2"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="F145" s="1">
         <v>1</v>
       </c>
@@ -3444,7 +3436,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F146" s="1">
         <v>1</v>
@@ -3453,7 +3445,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F147" s="1">
         <v>1</v>
@@ -3462,7 +3454,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F148" s="1">
         <v>1</v>
@@ -3471,7 +3463,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F149" s="1">
         <v>1</v>
@@ -3480,7 +3472,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>29</v>
+        <v>359</v>
       </c>
       <c r="F150" s="1">
         <v>1</v>
@@ -3489,7 +3481,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F151" s="1">
         <v>1</v>
@@ -3504,7 +3496,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F153" s="1">
         <v>1</v>
@@ -3537,7 +3529,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F158" s="1">
         <v>5</v>
@@ -3552,7 +3544,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F160" s="1">
         <v>5</v>
@@ -3573,7 +3565,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F163" s="1">
         <v>5</v>
@@ -3582,7 +3574,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="12" t="s">
-        <v>172</v>
+        <v>360</v>
       </c>
       <c r="F164" s="1">
         <v>5</v>
@@ -3591,7 +3583,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F165" s="1">
         <v>5</v>
@@ -4650,175 +4642,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE930D2-8264-4C13-BA9D-8D981850F45C}">
-  <dimension ref="A2:G10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="45">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="C5" s="45">
-        <f>A5/$A$10</f>
-        <v>0.125</v>
-      </c>
-      <c r="D5" s="45">
-        <f>C5*B5</f>
-        <v>0.1</v>
-      </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45">
-        <f>D5*$E$10</f>
-        <v>0.22535211267605637</v>
-      </c>
-      <c r="G5" s="45"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="45">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="C6" s="45">
-        <f>A6/$A$10</f>
-        <v>0.125</v>
-      </c>
-      <c r="D6" s="45">
-        <f t="shared" ref="D6:D8" si="0">C6*B6</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45">
-        <f t="shared" ref="F6:F10" si="1">D6*$E$10</f>
-        <v>0.16901408450704225</v>
-      </c>
-      <c r="G6" s="45"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="45">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="C7" s="45">
-        <f>A7/$A$10</f>
-        <v>0.125</v>
-      </c>
-      <c r="D7" s="45">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45">
-        <f t="shared" si="1"/>
-        <v>0.11267605633802819</v>
-      </c>
-      <c r="G7" s="45"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="45">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="C8" s="45">
-        <f>A8/$A$10</f>
-        <v>0.625</v>
-      </c>
-      <c r="D8" s="45">
-        <f t="shared" si="0"/>
-        <v>0.21875</v>
-      </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45">
-        <f t="shared" si="1"/>
-        <v>0.49295774647887325</v>
-      </c>
-      <c r="G8" s="45"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <f>SUM(A5:A8)</f>
-        <v>8</v>
-      </c>
-      <c r="C10" s="45">
-        <f>A10/$A$10</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <f>SUM(D5:D8)</f>
-        <v>0.44374999999999998</v>
-      </c>
-      <c r="E10" s="1">
-        <f>1/D10</f>
-        <v>2.2535211267605635</v>
-      </c>
-      <c r="F10" s="45">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214FE451-EC37-4DAA-9890-BA50B23E22A7}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -4838,7 +4661,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -4849,50 +4672,50 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B5" s="5">
         <v>4</v>
@@ -4906,7 +4729,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB02B54-F017-44DA-9118-EA158E750E4A}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -4925,7 +4748,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -4934,107 +4757,107 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>198</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -5046,11 +4869,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E13E4A5-10AD-4171-99FD-31881C0A6C11}">
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H10" sqref="H10:I10"/>
     </sheetView>
   </sheetViews>
@@ -5068,162 +4891,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
       <c r="AD1" s="19" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="38" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="37"/>
+      <c r="J3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="38" t="s">
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="38" t="s">
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" s="37"/>
+      <c r="X3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="38"/>
-      <c r="X3" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="39"/>
-      <c r="AB3" s="39"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
     </row>
     <row r="4" spans="1:30" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
       <c r="H4" s="33" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I4" s="33"/>
       <c r="J4" s="34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
       <c r="O4" s="35" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="P4" s="35"/>
       <c r="Q4" s="34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="R4" s="34"/>
       <c r="S4" s="34"/>
       <c r="T4" s="34"/>
       <c r="U4" s="34"/>
       <c r="V4" s="35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="W4" s="35"/>
       <c r="X4" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Y4" s="34"/>
       <c r="Z4" s="34"/>
@@ -5232,44 +5055,44 @@
     </row>
     <row r="5" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
       <c r="H5" s="33" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="I5" s="33"/>
       <c r="J5" s="34" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
       <c r="N5" s="34"/>
       <c r="O5" s="35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="P5" s="35"/>
       <c r="Q5" s="34" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="R5" s="34"/>
       <c r="S5" s="34"/>
       <c r="T5" s="34"/>
       <c r="U5" s="34"/>
       <c r="V5" s="35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="W5" s="35"/>
       <c r="X5" s="34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Y5" s="34"/>
       <c r="Z5" s="34"/>
@@ -5278,44 +5101,44 @@
     </row>
     <row r="6" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
       <c r="H6" s="33" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="I6" s="33"/>
       <c r="J6" s="34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
       <c r="N6" s="34"/>
       <c r="O6" s="35" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="P6" s="35"/>
       <c r="Q6" s="34" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="R6" s="34"/>
       <c r="S6" s="34"/>
       <c r="T6" s="34"/>
       <c r="U6" s="34"/>
       <c r="V6" s="35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="W6" s="35"/>
       <c r="X6" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Y6" s="34"/>
       <c r="Z6" s="34"/>
@@ -5324,44 +5147,44 @@
     </row>
     <row r="7" spans="1:30" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
       <c r="H7" s="33" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="I7" s="33"/>
       <c r="J7" s="34" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>
       <c r="N7" s="34"/>
       <c r="O7" s="35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P7" s="35"/>
       <c r="Q7" s="34" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="R7" s="34"/>
       <c r="S7" s="34"/>
       <c r="T7" s="34"/>
       <c r="U7" s="34"/>
       <c r="V7" s="35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="W7" s="35"/>
       <c r="X7" s="34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y7" s="34"/>
       <c r="Z7" s="34"/>
@@ -5370,11 +5193,11 @@
     </row>
     <row r="8" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -5388,22 +5211,22 @@
       <c r="M8" s="34"/>
       <c r="N8" s="34"/>
       <c r="O8" s="35" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="P8" s="35"/>
       <c r="Q8" s="34" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="R8" s="34"/>
       <c r="S8" s="34"/>
       <c r="T8" s="34"/>
       <c r="U8" s="34"/>
       <c r="V8" s="35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W8" s="35"/>
       <c r="X8" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Y8" s="34"/>
       <c r="Z8" s="34"/>
@@ -5419,33 +5242,33 @@
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
       <c r="H9" s="33" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="I9" s="33"/>
       <c r="J9" s="34" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
       <c r="M9" s="34"/>
       <c r="N9" s="34"/>
       <c r="O9" s="35" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="P9" s="35"/>
       <c r="Q9" s="34" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="R9" s="34"/>
       <c r="S9" s="34"/>
       <c r="T9" s="34"/>
       <c r="U9" s="34"/>
       <c r="V9" s="35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="W9" s="35"/>
       <c r="X9" s="34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Y9" s="34"/>
       <c r="Z9" s="34"/>
@@ -5454,11 +5277,11 @@
     </row>
     <row r="10" spans="1:30" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
@@ -5472,22 +5295,22 @@
       <c r="M10" s="34"/>
       <c r="N10" s="34"/>
       <c r="O10" s="35" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="P10" s="35"/>
       <c r="Q10" s="34" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="R10" s="34"/>
       <c r="S10" s="34"/>
       <c r="T10" s="34"/>
       <c r="U10" s="34"/>
       <c r="V10" s="35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W10" s="35"/>
       <c r="X10" s="34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Y10" s="34"/>
       <c r="Z10" s="34"/>
@@ -5496,44 +5319,44 @@
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
       <c r="H11" s="33" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="I11" s="33"/>
       <c r="J11" s="34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
       <c r="M11" s="34"/>
       <c r="N11" s="34"/>
       <c r="O11" s="35" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="P11" s="35"/>
       <c r="Q11" s="34" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="R11" s="34"/>
       <c r="S11" s="34"/>
       <c r="T11" s="34"/>
       <c r="U11" s="34"/>
       <c r="V11" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="W11" s="35"/>
       <c r="X11" s="34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Y11" s="34"/>
       <c r="Z11" s="34"/>
@@ -5543,17 +5366,17 @@
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="33"/>
       <c r="B12" s="33"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
       <c r="H12" s="33" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="I12" s="33"/>
       <c r="J12" s="34" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
@@ -5576,44 +5399,44 @@
     </row>
     <row r="13" spans="1:30" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B13" s="33"/>
-      <c r="C13" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
+      <c r="C13" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="33" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I13" s="33"/>
       <c r="J13" s="34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
       <c r="O13" s="35" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P13" s="35"/>
       <c r="Q13" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="R13" s="34"/>
       <c r="S13" s="34"/>
       <c r="T13" s="34"/>
       <c r="U13" s="34"/>
       <c r="V13" s="33" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="W13" s="33"/>
       <c r="X13" s="34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y13" s="34"/>
       <c r="Z13" s="34"/>
@@ -5622,16 +5445,16 @@
     </row>
     <row r="14" spans="1:30" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B14" s="33"/>
-      <c r="C14" s="36" t="s">
-        <v>238</v>
-      </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
+      <c r="C14" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
       <c r="J14" s="34"/>
@@ -5656,11 +5479,11 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B15" s="33"/>
-      <c r="C15" s="36" t="s">
-        <v>241</v>
+      <c r="C15" s="39" t="s">
+        <v>238</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
@@ -5690,7 +5513,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34"/>
@@ -6178,77 +6001,143 @@
     </row>
   </sheetData>
   <mergeCells count="236">
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:AB4"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:N2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="V1:AB2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="O1:U2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:AB5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:AB8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:AB7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:AB10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:U10"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:U34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:U33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:U32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:U31"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:U30"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:U29"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:U28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:U26"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:U24"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:U23"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="X22:AB22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:AB21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:U21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:U22"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="X20:AB20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="X19:AB19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:U19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:U20"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="X18:AB18"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:AB17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:U17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:U18"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="X13:AB13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="X16:AB16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="X15:AB15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:U16"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="H16:I16"/>
@@ -6273,147 +6162,81 @@
     <mergeCell ref="Q13:U13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:G14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:U10"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:AB7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:AB5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="H14:I14"/>
     <mergeCell ref="V13:W13"/>
     <mergeCell ref="J14:N14"/>
     <mergeCell ref="V14:W14"/>
     <mergeCell ref="X14:AB14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="X13:AB13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="X16:AB16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="X15:AB15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:U15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:U16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:AB18"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:AB17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:U17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:U18"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="X20:AB20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="X19:AB19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:U19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:U20"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="X22:AB22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:AB21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:U21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:U22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:U24"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:U23"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:U26"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:U25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:U28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:U30"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:U29"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:U32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:U31"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:U34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:U33"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:N2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="V1:AB2"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="O1:U2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:AB4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C15" r:id="rId1" xr:uid="{868F8F85-B252-4B04-B081-E9B23AD46A23}"/>
@@ -6425,7 +6248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1908B5E3-0D9D-48A8-894B-90B53E0249A0}">
   <dimension ref="A1:I26"/>
   <sheetViews>
@@ -6447,7 +6270,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="41" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -6459,19 +6282,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
@@ -6479,19 +6302,19 @@
     </row>
     <row r="3" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C3" s="21">
         <v>1</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F3" s="40"/>
       <c r="G3" s="40"/>
@@ -6499,16 +6322,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C4" s="21">
         <v>2</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E4" s="40"/>
       <c r="F4" s="40"/>
@@ -6535,19 +6358,19 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C8" s="21">
         <v>2</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="40"/>
@@ -6555,19 +6378,19 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C9" s="21">
         <v>1</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="40"/>
@@ -6575,7 +6398,7 @@
     </row>
     <row r="10" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>14</v>
@@ -6584,33 +6407,33 @@
         <v>2</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F10" s="40"/>
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
       <c r="I10" s="14" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C11" s="21">
         <v>2</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="40"/>
@@ -6618,19 +6441,19 @@
     </row>
     <row r="12" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C12" s="21">
         <v>3</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F12" s="40"/>
       <c r="G12" s="40"/>
@@ -6638,7 +6461,7 @@
     </row>
     <row r="13" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>14</v>
@@ -6647,10 +6470,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F13" s="40"/>
       <c r="G13" s="40"/>
@@ -6658,19 +6481,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C14" s="21">
         <v>1</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F14" s="40"/>
       <c r="G14" s="40"/>
@@ -6750,12 +6573,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E24:H24"/>
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="E8:H8"/>
@@ -6768,20 +6593,18 @@
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD47BAA-02B8-4E56-868D-4BC0DFE6F64A}">
   <dimension ref="A1:J30"/>
   <sheetViews>
@@ -6806,7 +6629,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="43" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -6817,99 +6640,99 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="44" t="s">
         <v>245</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>248</v>
       </c>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="I2" s="23" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
       <c r="I3" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>280</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
       <c r="J4" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E5" s="42"/>
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
       <c r="J5" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E6" s="42"/>
       <c r="F6" s="42"/>
@@ -6917,48 +6740,48 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D8" s="42"/>
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
       <c r="G8" s="42"/>
       <c r="I8" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
       <c r="J9" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -6975,39 +6798,39 @@
     </row>
     <row r="12" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D12" s="42" t="s">
         <v>282</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>285</v>
       </c>
       <c r="E12" s="42"/>
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
       <c r="I12" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -7015,16 +6838,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D14" s="42" t="s">
         <v>316</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>319</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -7044,16 +6867,16 @@
     </row>
     <row r="17" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D17" s="40" t="s">
         <v>296</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>299</v>
       </c>
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
@@ -7139,23 +6962,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="D20:G20"/>
@@ -7168,6 +6974,23 @@
     <mergeCell ref="D27:G27"/>
     <mergeCell ref="D28:G28"/>
     <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
minor work with sizes
</commit_message>
<xml_diff>
--- a/plans/todo.xlsx
+++ b/plans/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edsquid\Documents\Personal Projects\Business\RogueLikeGame\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B346AB-469B-4F22-8CD2-84538FF729F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6973DD4-75AF-49DA-8CDA-AFC8AF0AE1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="1395" windowWidth="16215" windowHeight="13335" tabRatio="509" activeTab="3" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
+    <workbookView xWindow="38355" yWindow="165" windowWidth="16215" windowHeight="13335" tabRatio="509" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="371">
   <si>
     <t>Max Lives</t>
   </si>
@@ -1140,6 +1140,21 @@
   </si>
   <si>
     <t>emporwed</t>
+  </si>
+  <si>
+    <t>Elemental effects/explosions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if frozen, shoot out ice </t>
+  </si>
+  <si>
+    <t>if on fire, explode</t>
+  </si>
+  <si>
+    <t>if zaped, chain lightning from corpse</t>
+  </si>
+  <si>
+    <t>increase chance to burn/zap/etc</t>
   </si>
 </sst>
 </file>
@@ -1474,6 +1489,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1502,19 +1518,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1525,8 +1538,11 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1543,7 +1559,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1861,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CE061F-AFA4-4B9D-BFD1-A05915568E6D}">
   <dimension ref="A1:H355"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,27 +1894,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="9" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="11" t="s">
         <v>166</v>
       </c>
@@ -1929,15 +1944,15 @@
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2445,15 +2460,15 @@
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -2594,15 +2609,15 @@
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
@@ -3351,21 +3366,36 @@
       <c r="G137" s="2"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>366</v>
+      </c>
       <c r="G138" s="2"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>367</v>
+      </c>
       <c r="G139" s="2"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>368</v>
+      </c>
       <c r="F140" s="1">
         <v>5</v>
       </c>
       <c r="G140" s="2"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>369</v>
+      </c>
       <c r="G141" s="2"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>370</v>
+      </c>
       <c r="G142" s="2"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -3417,15 +3447,15 @@
       <c r="G150" s="4"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A151" s="25" t="s">
+      <c r="A151" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B151" s="25"/>
-      <c r="C151" s="25"/>
-      <c r="D151" s="25"/>
-      <c r="E151" s="25"/>
-      <c r="F151" s="25"/>
-      <c r="G151" s="25"/>
+      <c r="B151" s="26"/>
+      <c r="C151" s="26"/>
+      <c r="D151" s="26"/>
+      <c r="E151" s="26"/>
+      <c r="F151" s="26"/>
+      <c r="G151" s="26"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="16" t="s">
@@ -4749,15 +4779,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -4836,13 +4866,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -4962,13 +4992,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF194B0-B750-47C3-A920-7899813FCE3E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="47"/>
+    <col min="1" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5116,1147 +5146,1091 @@
       <c r="AB3" s="40"/>
     </row>
     <row r="4" spans="1:30" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="41" t="s">
         <v>362</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="42" t="s">
         <v>363</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="37" t="s">
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="34" t="s">
         <v>312</v>
       </c>
-      <c r="I4" s="37"/>
-      <c r="J4" s="34" t="s">
+      <c r="I4" s="34"/>
+      <c r="J4" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="33" t="s">
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="36" t="s">
         <v>325</v>
       </c>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="34" t="s">
+      <c r="P4" s="36"/>
+      <c r="Q4" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="33" t="s">
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
+      <c r="V4" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="W4" s="33"/>
-      <c r="X4" s="34" t="s">
+      <c r="W4" s="36"/>
+      <c r="X4" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="Y4" s="34"/>
-      <c r="Z4" s="34"/>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="34"/>
+      <c r="Y4" s="35"/>
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="35"/>
     </row>
     <row r="5" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="34" t="s">
         <v>361</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="34" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="37" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="34" t="s">
         <v>313</v>
       </c>
-      <c r="I5" s="37"/>
-      <c r="J5" s="34" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="35" t="s">
         <v>314</v>
       </c>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="33" t="s">
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="34" t="s">
+      <c r="P5" s="36"/>
+      <c r="Q5" s="35" t="s">
         <v>234</v>
       </c>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="33" t="s">
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="W5" s="33"/>
-      <c r="X5" s="34" t="s">
+      <c r="W5" s="36"/>
+      <c r="X5" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="Y5" s="34"/>
-      <c r="Z5" s="34"/>
-      <c r="AA5" s="34"/>
-      <c r="AB5" s="34"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="35"/>
+      <c r="AA5" s="35"/>
+      <c r="AB5" s="35"/>
     </row>
     <row r="6" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="34" t="s">
         <v>364</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="34" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="37" t="s">
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="I6" s="37"/>
-      <c r="J6" s="34" t="s">
+      <c r="I6" s="34"/>
+      <c r="J6" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="33" t="s">
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="34" t="s">
+      <c r="P6" s="36"/>
+      <c r="Q6" s="35" t="s">
         <v>234</v>
       </c>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="33" t="s">
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="W6" s="33"/>
-      <c r="X6" s="34" t="s">
+      <c r="W6" s="36"/>
+      <c r="X6" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="Y6" s="34"/>
-      <c r="Z6" s="34"/>
-      <c r="AA6" s="34"/>
-      <c r="AB6" s="34"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="35"/>
+      <c r="AB6" s="35"/>
     </row>
     <row r="7" spans="1:30" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="37" t="s">
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="34" t="s">
         <v>324</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="34" t="s">
+      <c r="I7" s="34"/>
+      <c r="J7" s="35" t="s">
         <v>360</v>
       </c>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="33" t="s">
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="34" t="s">
+      <c r="P7" s="36"/>
+      <c r="Q7" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="R7" s="34"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="34"/>
-      <c r="V7" s="33" t="s">
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="W7" s="33"/>
-      <c r="X7" s="34" t="s">
+      <c r="W7" s="36"/>
+      <c r="X7" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="Y7" s="34"/>
-      <c r="Z7" s="34"/>
-      <c r="AA7" s="34"/>
-      <c r="AB7" s="34"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="35"/>
+      <c r="AB7" s="35"/>
     </row>
     <row r="8" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="34"/>
+      <c r="C8" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="33" t="s">
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="36" t="s">
         <v>330</v>
       </c>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="34" t="s">
+      <c r="P8" s="36"/>
+      <c r="Q8" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="R8" s="34"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="34"/>
-      <c r="V8" s="33" t="s">
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="W8" s="33"/>
-      <c r="X8" s="34" t="s">
+      <c r="W8" s="36"/>
+      <c r="X8" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="Y8" s="34"/>
-      <c r="Z8" s="34"/>
-      <c r="AA8" s="34"/>
-      <c r="AB8" s="34"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="35"/>
+      <c r="AA8" s="35"/>
+      <c r="AB8" s="35"/>
     </row>
     <row r="9" spans="1:30" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="34" t="s">
         <v>328</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="34" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="37" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="34" t="s">
         <v>323</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="34" t="s">
+      <c r="I9" s="34"/>
+      <c r="J9" s="35" t="s">
         <v>326</v>
       </c>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="33" t="s">
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="36" t="s">
         <v>319</v>
       </c>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="34" t="s">
+      <c r="P9" s="36"/>
+      <c r="Q9" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="34"/>
-      <c r="V9" s="33" t="s">
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="W9" s="33"/>
-      <c r="X9" s="34" t="s">
+      <c r="W9" s="36"/>
+      <c r="X9" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="Y9" s="34"/>
-      <c r="Z9" s="34"/>
-      <c r="AA9" s="34"/>
-      <c r="AB9" s="34"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35"/>
+      <c r="AA9" s="35"/>
+      <c r="AB9" s="35"/>
     </row>
     <row r="10" spans="1:30" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="33" t="s">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="36" t="s">
         <v>316</v>
       </c>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="34" t="s">
+      <c r="P10" s="36"/>
+      <c r="Q10" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="34"/>
-      <c r="V10" s="33" t="s">
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35"/>
+      <c r="V10" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="W10" s="33"/>
-      <c r="X10" s="34" t="s">
+      <c r="W10" s="36"/>
+      <c r="X10" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="Y10" s="34"/>
-      <c r="Z10" s="34"/>
-      <c r="AA10" s="34"/>
-      <c r="AB10" s="34"/>
+      <c r="Y10" s="35"/>
+      <c r="Z10" s="35"/>
+      <c r="AA10" s="35"/>
+      <c r="AB10" s="35"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="34" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="37" t="s">
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="I11" s="37"/>
-      <c r="J11" s="34" t="s">
+      <c r="I11" s="34"/>
+      <c r="J11" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="33" t="s">
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="36" t="s">
         <v>318</v>
       </c>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="34" t="s">
+      <c r="P11" s="36"/>
+      <c r="Q11" s="35" t="s">
         <v>359</v>
       </c>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="34"/>
-      <c r="U11" s="34"/>
-      <c r="V11" s="33" t="s">
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="W11" s="33"/>
-      <c r="X11" s="34" t="s">
+      <c r="W11" s="36"/>
+      <c r="X11" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="Y11" s="34"/>
-      <c r="Z11" s="34"/>
-      <c r="AA11" s="34"/>
-      <c r="AB11" s="34"/>
+      <c r="Y11" s="35"/>
+      <c r="Z11" s="35"/>
+      <c r="AA11" s="35"/>
+      <c r="AB11" s="35"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="34" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="37" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="34" t="s">
+      <c r="I12" s="34"/>
+      <c r="J12" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
-      <c r="T12" s="34"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="33"/>
-      <c r="W12" s="33"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="34"/>
-      <c r="Z12" s="34"/>
-      <c r="AA12" s="34"/>
-      <c r="AB12" s="34"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="35"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="35"/>
+      <c r="Y12" s="35"/>
+      <c r="Z12" s="35"/>
+      <c r="AA12" s="35"/>
+      <c r="AB12" s="35"/>
     </row>
     <row r="13" spans="1:30" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="37" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="34" t="s">
+      <c r="I13" s="34"/>
+      <c r="J13" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="33" t="s">
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="36" t="s">
         <v>320</v>
       </c>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="34" t="s">
+      <c r="P13" s="36"/>
+      <c r="Q13" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="34"/>
-      <c r="U13" s="34"/>
-      <c r="V13" s="37" t="s">
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="35"/>
+      <c r="U13" s="35"/>
+      <c r="V13" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="W13" s="37"/>
-      <c r="X13" s="34" t="s">
+      <c r="W13" s="34"/>
+      <c r="X13" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="34"/>
-      <c r="AA13" s="34"/>
-      <c r="AB13" s="34"/>
+      <c r="Y13" s="35"/>
+      <c r="Z13" s="35"/>
+      <c r="AA13" s="35"/>
+      <c r="AB13" s="35"/>
     </row>
     <row r="14" spans="1:30" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="41" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
-      <c r="T14" s="34"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="33"/>
-      <c r="W14" s="33"/>
-      <c r="X14" s="34"/>
-      <c r="Y14" s="34"/>
-      <c r="Z14" s="34"/>
-      <c r="AA14" s="34"/>
-      <c r="AB14" s="34"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="35"/>
+      <c r="Y14" s="35"/>
+      <c r="Z14" s="35"/>
+      <c r="AA14" s="35"/>
+      <c r="AB14" s="35"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="41" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
-      <c r="U15" s="34"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="33"/>
-      <c r="X15" s="34"/>
-      <c r="Y15" s="34"/>
-      <c r="Z15" s="34"/>
-      <c r="AA15" s="34"/>
-      <c r="AB15" s="34"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="35"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="36"/>
+      <c r="X15" s="35"/>
+      <c r="Y15" s="35"/>
+      <c r="Z15" s="35"/>
+      <c r="AA15" s="35"/>
+      <c r="AB15" s="35"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="41" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="34"/>
-      <c r="U16" s="34"/>
-      <c r="V16" s="33"/>
-      <c r="W16" s="33"/>
-      <c r="X16" s="34"/>
-      <c r="Y16" s="34"/>
-      <c r="Z16" s="34"/>
-      <c r="AA16" s="34"/>
-      <c r="AB16" s="34"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="35"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="35"/>
+      <c r="Y16" s="35"/>
+      <c r="Z16" s="35"/>
+      <c r="AA16" s="35"/>
+      <c r="AB16" s="35"/>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
-      <c r="T17" s="34"/>
-      <c r="U17" s="34"/>
-      <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
-      <c r="X17" s="34"/>
-      <c r="Y17" s="34"/>
-      <c r="Z17" s="34"/>
-      <c r="AA17" s="34"/>
-      <c r="AB17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="35"/>
+      <c r="Y17" s="35"/>
+      <c r="Z17" s="35"/>
+      <c r="AA17" s="35"/>
+      <c r="AB17" s="35"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="34"/>
-      <c r="U18" s="34"/>
-      <c r="V18" s="33"/>
-      <c r="W18" s="33"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="34"/>
-      <c r="Z18" s="34"/>
-      <c r="AA18" s="34"/>
-      <c r="AB18" s="34"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="35"/>
+      <c r="Y18" s="35"/>
+      <c r="Z18" s="35"/>
+      <c r="AA18" s="35"/>
+      <c r="AB18" s="35"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="34"/>
-      <c r="T19" s="34"/>
-      <c r="U19" s="34"/>
-      <c r="V19" s="33"/>
-      <c r="W19" s="33"/>
-      <c r="X19" s="34"/>
-      <c r="Y19" s="34"/>
-      <c r="Z19" s="34"/>
-      <c r="AA19" s="34"/>
-      <c r="AB19" s="34"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="35"/>
+      <c r="U19" s="35"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="35"/>
+      <c r="Y19" s="35"/>
+      <c r="Z19" s="35"/>
+      <c r="AA19" s="35"/>
+      <c r="AB19" s="35"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="33"/>
-      <c r="W20" s="33"/>
-      <c r="X20" s="34"/>
-      <c r="Y20" s="34"/>
-      <c r="Z20" s="34"/>
-      <c r="AA20" s="34"/>
-      <c r="AB20" s="34"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="35"/>
+      <c r="Y20" s="35"/>
+      <c r="Z20" s="35"/>
+      <c r="AA20" s="35"/>
+      <c r="AB20" s="35"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="34"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="33"/>
-      <c r="W21" s="33"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="34"/>
-      <c r="Z21" s="34"/>
-      <c r="AA21" s="34"/>
-      <c r="AB21" s="34"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
+      <c r="X21" s="35"/>
+      <c r="Y21" s="35"/>
+      <c r="Z21" s="35"/>
+      <c r="AA21" s="35"/>
+      <c r="AB21" s="35"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="34"/>
-      <c r="T22" s="34"/>
-      <c r="U22" s="34"/>
-      <c r="V22" s="33"/>
-      <c r="W22" s="33"/>
-      <c r="X22" s="34"/>
-      <c r="Y22" s="34"/>
-      <c r="Z22" s="34"/>
-      <c r="AA22" s="34"/>
-      <c r="AB22" s="34"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
+      <c r="V22" s="36"/>
+      <c r="W22" s="36"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="35"/>
+      <c r="Z22" s="35"/>
+      <c r="AA22" s="35"/>
+      <c r="AB22" s="35"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="34"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="34"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="35"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="34"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="34"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="34"/>
-      <c r="T25" s="34"/>
-      <c r="U25" s="34"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="35"/>
+      <c r="U25" s="35"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="33"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="34"/>
-      <c r="U26" s="34"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35"/>
+      <c r="T26" s="35"/>
+      <c r="U26" s="35"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="34"/>
-      <c r="T27" s="34"/>
-      <c r="U27" s="34"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="35"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
-      <c r="S28" s="34"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="34"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="34"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="34"/>
-      <c r="R29" s="34"/>
-      <c r="S29" s="34"/>
-      <c r="T29" s="34"/>
-      <c r="U29" s="34"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="35"/>
+      <c r="S29" s="35"/>
+      <c r="T29" s="35"/>
+      <c r="U29" s="35"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="34"/>
-      <c r="S30" s="34"/>
-      <c r="T30" s="34"/>
-      <c r="U30" s="34"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="35"/>
+      <c r="S30" s="35"/>
+      <c r="T30" s="35"/>
+      <c r="U30" s="35"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="34"/>
-      <c r="R31" s="34"/>
-      <c r="S31" s="34"/>
-      <c r="T31" s="34"/>
-      <c r="U31" s="34"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="35"/>
+      <c r="S31" s="35"/>
+      <c r="T31" s="35"/>
+      <c r="U31" s="35"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="33"/>
-      <c r="P32" s="33"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
-      <c r="S32" s="34"/>
-      <c r="T32" s="34"/>
-      <c r="U32" s="34"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="35"/>
+      <c r="R32" s="35"/>
+      <c r="S32" s="35"/>
+      <c r="T32" s="35"/>
+      <c r="U32" s="35"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="34"/>
-      <c r="S33" s="34"/>
-      <c r="T33" s="34"/>
-      <c r="U33" s="34"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="34"/>
+      <c r="P33" s="34"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="35"/>
+      <c r="U33" s="35"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="37"/>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="34"/>
-      <c r="S34" s="34"/>
-      <c r="T34" s="34"/>
-      <c r="U34" s="34"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="34"/>
+      <c r="P34" s="34"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="35"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="238">
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:U34"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:U33"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:U32"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:U31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:U30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:U29"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:U28"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:U26"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:U25"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:U24"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:U23"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="X22:AB22"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:AB21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:U21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:U22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="X20:AB20"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="X19:AB19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:U19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:U20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:AB18"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:AB17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:U17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:U18"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="X15:AB15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:U15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:U16"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="X14:AB14"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:AB5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:AB4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:N2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="V1:AB2"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="O1:U2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:AB7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:U10"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="X11:AB11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:U11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:G13"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="J16:N16"/>
     <mergeCell ref="V12:W12"/>
@@ -6281,85 +6255,141 @@
     <mergeCell ref="X16:AB16"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:G16"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:AB10"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:U10"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="X11:AB11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:U11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:AB8"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:AB7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:N2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="V1:AB2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="O1:U2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:AB5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:AB4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="X15:AB15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:U16"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="X14:AB14"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="X18:AB18"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:AB17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:U17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:U18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="X20:AB20"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="X19:AB19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:U19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:U20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="X22:AB22"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:AB21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:U21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:U22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:U24"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:U23"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:U26"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:U28"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:U30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:U29"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:U32"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:U31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:U34"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:U33"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:G33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C16" r:id="rId1" xr:uid="{868F8F85-B252-4B04-B081-E9B23AD46A23}"/>
@@ -6392,16 +6422,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -6416,12 +6446,12 @@
       <c r="D2" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="35" t="s">
         <v>240</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -6436,12 +6466,12 @@
       <c r="D3" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -6456,28 +6486,28 @@
       <c r="D4" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
@@ -6492,12 +6522,12 @@
       <c r="D8" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="43" t="s">
         <v>285</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
@@ -6512,12 +6542,12 @@
       <c r="D9" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
@@ -6532,12 +6562,12 @@
       <c r="D10" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
       <c r="I10" s="14" t="s">
         <v>282</v>
       </c>
@@ -6555,12 +6585,12 @@
       <c r="D11" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="43" t="s">
         <v>255</v>
       </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
     </row>
     <row r="12" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -6575,12 +6605,12 @@
       <c r="D12" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="43" t="s">
         <v>259</v>
       </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
@@ -6595,12 +6625,12 @@
       <c r="D13" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
@@ -6615,95 +6645,93 @@
       <c r="D14" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="43" t="s">
         <v>287</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
     </row>
     <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
     </row>
     <row r="19" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
     </row>
     <row r="20" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
     </row>
     <row r="22" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
     </row>
     <row r="23" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
     </row>
     <row r="26" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="E8:H8"/>
@@ -6716,12 +6744,14 @@
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E24:H24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6751,15 +6781,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -6771,12 +6801,12 @@
       <c r="C2" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
       <c r="I2" s="23" t="s">
         <v>294</v>
       </c>
@@ -6791,12 +6821,12 @@
       <c r="C3" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
       <c r="I3" s="5" t="s">
         <v>295</v>
       </c>
@@ -6814,12 +6844,12 @@
       <c r="C4" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="45" t="s">
         <v>271</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="5" t="s">
         <v>298</v>
       </c>
@@ -6834,12 +6864,12 @@
       <c r="C5" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
       <c r="J5" s="5" t="s">
         <v>299</v>
       </c>
@@ -6854,12 +6884,12 @@
       <c r="C6" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
@@ -6868,10 +6898,10 @@
       <c r="A8" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
       <c r="I8" s="5" t="s">
         <v>164</v>
       </c>
@@ -6889,12 +6919,12 @@
       <c r="C9" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
       <c r="J9" s="5" t="s">
         <v>304</v>
       </c>
@@ -6911,10 +6941,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
     </row>
     <row r="12" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -6926,12 +6956,12 @@
       <c r="C12" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
       <c r="I12" s="5" t="s">
         <v>306</v>
       </c>
@@ -6949,12 +6979,12 @@
       <c r="C13" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="45" t="s">
         <v>280</v>
       </c>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -6966,24 +6996,24 @@
       <c r="C14" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="45" t="s">
         <v>311</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
     </row>
     <row r="17" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -6995,93 +7025,109 @@
       <c r="C17" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="43" t="s">
         <v>291</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="D20:G20"/>
@@ -7094,22 +7140,6 @@
     <mergeCell ref="D27:G27"/>
     <mergeCell ref="D28:G28"/>
     <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Delete unused weapon images and make changes to weapon rendering and UI
</commit_message>
<xml_diff>
--- a/plans/todo.xlsx
+++ b/plans/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edsquid\Documents\Personal Projects\Business\RogueLikeGame\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A498F03B-841C-4664-B0B3-0E35CCD02BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D2C425-54E9-4A23-A338-B6D4480EA510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="509" activeTab="3" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
+    <workbookView xWindow="30315" yWindow="2970" windowWidth="17415" windowHeight="13335" tabRatio="509" firstSheet="2" activeTab="4" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="3" r:id="rId1"/>
@@ -1466,7 +1466,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1578,6 +1578,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1696,7 +1702,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1791,19 +1797,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1814,8 +1817,11 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1833,6 +1839,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5520,7 +5532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF194B0-B750-47C3-A920-7899813FCE3E}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
@@ -5641,8 +5653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E13E4A5-10AD-4171-99FD-31881C0A6C11}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12:I12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5661,138 +5673,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54" t="s">
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54" t="s">
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
       <c r="AD1" s="18" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="55" t="s">
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="55"/>
-      <c r="J3" s="56" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="55" t="s">
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="56" t="s">
+      <c r="P3" s="54"/>
+      <c r="Q3" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="55" t="s">
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="55"/>
-      <c r="X3" s="56" t="s">
+      <c r="W3" s="54"/>
+      <c r="X3" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="56"/>
+      <c r="Y3" s="55"/>
+      <c r="Z3" s="55"/>
+      <c r="AA3" s="55"/>
+      <c r="AB3" s="55"/>
     </row>
     <row r="4" spans="1:30" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="56" t="s">
         <v>346</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="56"/>
+      <c r="C4" s="57" t="s">
         <v>347</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="53" t="s">
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="64" t="s">
         <v>298</v>
       </c>
-      <c r="I4" s="53"/>
+      <c r="I4" s="64"/>
       <c r="J4" s="50" t="s">
         <v>36</v>
       </c>
@@ -5800,10 +5812,10 @@
       <c r="L4" s="50"/>
       <c r="M4" s="50"/>
       <c r="N4" s="50"/>
-      <c r="O4" s="49" t="s">
+      <c r="O4" s="51" t="s">
         <v>309</v>
       </c>
-      <c r="P4" s="49"/>
+      <c r="P4" s="51"/>
       <c r="Q4" s="50" t="s">
         <v>151</v>
       </c>
@@ -5811,10 +5823,10 @@
       <c r="S4" s="50"/>
       <c r="T4" s="50"/>
       <c r="U4" s="50"/>
-      <c r="V4" s="49" t="s">
+      <c r="V4" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="W4" s="49"/>
+      <c r="W4" s="51"/>
       <c r="X4" s="50" t="s">
         <v>42</v>
       </c>
@@ -5824,10 +5836,10 @@
       <c r="AB4" s="50"/>
     </row>
     <row r="5" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="49" t="s">
         <v>345</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="50" t="s">
         <v>35</v>
       </c>
@@ -5835,10 +5847,10 @@
       <c r="E5" s="50"/>
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="64" t="s">
         <v>299</v>
       </c>
-      <c r="I5" s="53"/>
+      <c r="I5" s="64"/>
       <c r="J5" s="50" t="s">
         <v>300</v>
       </c>
@@ -5846,10 +5858,10 @@
       <c r="L5" s="50"/>
       <c r="M5" s="50"/>
       <c r="N5" s="50"/>
-      <c r="O5" s="49" t="s">
+      <c r="O5" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="P5" s="49"/>
+      <c r="P5" s="51"/>
       <c r="Q5" s="50" t="s">
         <v>224</v>
       </c>
@@ -5857,10 +5869,10 @@
       <c r="S5" s="50"/>
       <c r="T5" s="50"/>
       <c r="U5" s="50"/>
-      <c r="V5" s="49" t="s">
+      <c r="V5" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="W5" s="49"/>
+      <c r="W5" s="51"/>
       <c r="X5" s="50" t="s">
         <v>45</v>
       </c>
@@ -5870,10 +5882,10 @@
       <c r="AB5" s="50"/>
     </row>
     <row r="6" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="49" t="s">
         <v>348</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="50" t="s">
         <v>213</v>
       </c>
@@ -5881,10 +5893,10 @@
       <c r="E6" s="50"/>
       <c r="F6" s="50"/>
       <c r="G6" s="50"/>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="64" t="s">
         <v>301</v>
       </c>
-      <c r="I6" s="53"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="50" t="s">
         <v>38</v>
       </c>
@@ -5892,10 +5904,10 @@
       <c r="L6" s="50"/>
       <c r="M6" s="50"/>
       <c r="N6" s="50"/>
-      <c r="O6" s="49" t="s">
+      <c r="O6" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="P6" s="49"/>
+      <c r="P6" s="51"/>
       <c r="Q6" s="50" t="s">
         <v>224</v>
       </c>
@@ -5903,8 +5915,8 @@
       <c r="S6" s="50"/>
       <c r="T6" s="50"/>
       <c r="U6" s="50"/>
-      <c r="V6" s="49"/>
-      <c r="W6" s="49"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="51"/>
       <c r="X6" s="50"/>
       <c r="Y6" s="50"/>
       <c r="Z6" s="50"/>
@@ -5912,10 +5924,10 @@
       <c r="AB6" s="50"/>
     </row>
     <row r="7" spans="1:30" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="50" t="s">
         <v>39</v>
       </c>
@@ -5923,10 +5935,10 @@
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="65" t="s">
         <v>308</v>
       </c>
-      <c r="I7" s="53"/>
+      <c r="I7" s="65"/>
       <c r="J7" s="50" t="s">
         <v>344</v>
       </c>
@@ -5934,10 +5946,10 @@
       <c r="L7" s="50"/>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
-      <c r="O7" s="49" t="s">
+      <c r="O7" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="P7" s="49"/>
+      <c r="P7" s="51"/>
       <c r="Q7" s="50" t="s">
         <v>225</v>
       </c>
@@ -5945,10 +5957,10 @@
       <c r="S7" s="50"/>
       <c r="T7" s="50"/>
       <c r="U7" s="50"/>
-      <c r="V7" s="49" t="s">
+      <c r="V7" s="51" t="s">
         <v>342</v>
       </c>
-      <c r="W7" s="49"/>
+      <c r="W7" s="51"/>
       <c r="X7" s="50" t="s">
         <v>46</v>
       </c>
@@ -5958,10 +5970,10 @@
       <c r="AB7" s="50"/>
     </row>
     <row r="8" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="53"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="50" t="s">
         <v>34</v>
       </c>
@@ -5969,17 +5981,17 @@
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="50"/>
       <c r="K8" s="50"/>
       <c r="L8" s="50"/>
       <c r="M8" s="50"/>
       <c r="N8" s="50"/>
-      <c r="O8" s="49" t="s">
+      <c r="O8" s="51" t="s">
         <v>314</v>
       </c>
-      <c r="P8" s="49"/>
+      <c r="P8" s="51"/>
       <c r="Q8" s="50" t="s">
         <v>225</v>
       </c>
@@ -5987,10 +5999,10 @@
       <c r="S8" s="50"/>
       <c r="T8" s="50"/>
       <c r="U8" s="50"/>
-      <c r="V8" s="49" t="s">
+      <c r="V8" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="W8" s="49"/>
+      <c r="W8" s="51"/>
       <c r="X8" s="50" t="s">
         <v>42</v>
       </c>
@@ -6000,10 +6012,10 @@
       <c r="AB8" s="50"/>
     </row>
     <row r="9" spans="1:30" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="49" t="s">
         <v>312</v>
       </c>
-      <c r="B9" s="53"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="50" t="s">
         <v>212</v>
       </c>
@@ -6011,10 +6023,10 @@
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
-      <c r="H9" s="53" t="s">
+      <c r="H9" s="64" t="s">
         <v>307</v>
       </c>
-      <c r="I9" s="53"/>
+      <c r="I9" s="64"/>
       <c r="J9" s="50" t="s">
         <v>310</v>
       </c>
@@ -6022,10 +6034,10 @@
       <c r="L9" s="50"/>
       <c r="M9" s="50"/>
       <c r="N9" s="50"/>
-      <c r="O9" s="49" t="s">
+      <c r="O9" s="51" t="s">
         <v>303</v>
       </c>
-      <c r="P9" s="49"/>
+      <c r="P9" s="51"/>
       <c r="Q9" s="50" t="s">
         <v>268</v>
       </c>
@@ -6033,10 +6045,10 @@
       <c r="S9" s="50"/>
       <c r="T9" s="50"/>
       <c r="U9" s="50"/>
-      <c r="V9" s="49" t="s">
+      <c r="V9" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="W9" s="49"/>
+      <c r="W9" s="51"/>
       <c r="X9" s="50" t="s">
         <v>49</v>
       </c>
@@ -6046,17 +6058,17 @@
       <c r="AB9" s="50"/>
     </row>
     <row r="10" spans="1:30" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
-      <c r="B10" s="53"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="50"/>
       <c r="D10" s="50"/>
       <c r="E10" s="50"/>
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
-      <c r="H10" s="53" t="s">
+      <c r="H10" s="64" t="s">
         <v>433</v>
       </c>
-      <c r="I10" s="53"/>
+      <c r="I10" s="64"/>
       <c r="J10" s="50" t="s">
         <v>434</v>
       </c>
@@ -6064,10 +6076,10 @@
       <c r="L10" s="50"/>
       <c r="M10" s="50"/>
       <c r="N10" s="50"/>
-      <c r="O10" s="49" t="s">
+      <c r="O10" s="51" t="s">
         <v>435</v>
       </c>
-      <c r="P10" s="49"/>
+      <c r="P10" s="51"/>
       <c r="Q10" s="50" t="s">
         <v>436</v>
       </c>
@@ -6075,10 +6087,10 @@
       <c r="S10" s="50"/>
       <c r="T10" s="50"/>
       <c r="U10" s="50"/>
-      <c r="V10" s="49" t="s">
+      <c r="V10" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="W10" s="49"/>
+      <c r="W10" s="51"/>
       <c r="X10" s="50" t="s">
         <v>52</v>
       </c>
@@ -6088,10 +6100,10 @@
       <c r="AB10" s="50"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="53"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="50" t="s">
         <v>40</v>
       </c>
@@ -6099,10 +6111,10 @@
       <c r="E11" s="50"/>
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
-      <c r="H11" s="53" t="s">
+      <c r="H11" s="65" t="s">
         <v>306</v>
       </c>
-      <c r="I11" s="53"/>
+      <c r="I11" s="65"/>
       <c r="J11" s="50" t="s">
         <v>41</v>
       </c>
@@ -6110,10 +6122,10 @@
       <c r="L11" s="50"/>
       <c r="M11" s="50"/>
       <c r="N11" s="50"/>
-      <c r="O11" s="49" t="s">
+      <c r="O11" s="51" t="s">
         <v>302</v>
       </c>
-      <c r="P11" s="49"/>
+      <c r="P11" s="51"/>
       <c r="Q11" s="50" t="s">
         <v>343</v>
       </c>
@@ -6121,10 +6133,10 @@
       <c r="S11" s="50"/>
       <c r="T11" s="50"/>
       <c r="U11" s="50"/>
-      <c r="V11" s="49" t="s">
+      <c r="V11" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="W11" s="49"/>
+      <c r="W11" s="51"/>
       <c r="X11" s="50" t="s">
         <v>438</v>
       </c>
@@ -6134,17 +6146,17 @@
       <c r="AB11" s="50"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="50"/>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
-      <c r="H12" s="53" t="s">
+      <c r="H12" s="64" t="s">
         <v>305</v>
       </c>
-      <c r="I12" s="53"/>
+      <c r="I12" s="64"/>
       <c r="J12" s="50" t="s">
         <v>211</v>
       </c>
@@ -6152,15 +6164,15 @@
       <c r="L12" s="50"/>
       <c r="M12" s="50"/>
       <c r="N12" s="50"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="49"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
       <c r="Q12" s="50"/>
       <c r="R12" s="50"/>
       <c r="S12" s="50"/>
       <c r="T12" s="50"/>
       <c r="U12" s="50"/>
-      <c r="V12" s="49"/>
-      <c r="W12" s="49"/>
+      <c r="V12" s="51"/>
+      <c r="W12" s="51"/>
       <c r="X12" s="50"/>
       <c r="Y12" s="50"/>
       <c r="Z12" s="50"/>
@@ -6168,17 +6180,17 @@
       <c r="AB12" s="50"/>
     </row>
     <row r="13" spans="1:30" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="53" t="s">
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="64" t="s">
         <v>311</v>
       </c>
-      <c r="I13" s="53"/>
+      <c r="I13" s="64"/>
       <c r="J13" s="50" t="s">
         <v>37</v>
       </c>
@@ -6186,10 +6198,10 @@
       <c r="L13" s="50"/>
       <c r="M13" s="50"/>
       <c r="N13" s="50"/>
-      <c r="O13" s="49" t="s">
+      <c r="O13" s="51" t="s">
         <v>304</v>
       </c>
-      <c r="P13" s="49"/>
+      <c r="P13" s="51"/>
       <c r="Q13" s="50" t="s">
         <v>155</v>
       </c>
@@ -6197,10 +6209,10 @@
       <c r="S13" s="50"/>
       <c r="T13" s="50"/>
       <c r="U13" s="50"/>
-      <c r="V13" s="53" t="s">
+      <c r="V13" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="W13" s="53"/>
+      <c r="W13" s="49"/>
       <c r="X13" s="50" t="s">
         <v>46</v>
       </c>
@@ -6210,37 +6222,37 @@
       <c r="AB13" s="50"/>
     </row>
     <row r="14" spans="1:30" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="49" t="s">
         <v>218</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="57" t="s">
+      <c r="B14" s="49"/>
+      <c r="C14" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
       <c r="L14" s="50"/>
       <c r="M14" s="50"/>
       <c r="N14" s="50"/>
-      <c r="O14" s="49" t="s">
+      <c r="O14" s="51" t="s">
         <v>437</v>
       </c>
-      <c r="P14" s="49"/>
+      <c r="P14" s="51"/>
       <c r="Q14" s="50"/>
       <c r="R14" s="50"/>
       <c r="S14" s="50"/>
       <c r="T14" s="50"/>
       <c r="U14" s="50"/>
-      <c r="V14" s="49" t="s">
+      <c r="V14" s="51" t="s">
         <v>439</v>
       </c>
-      <c r="W14" s="49"/>
+      <c r="W14" s="51"/>
       <c r="X14" s="50"/>
       <c r="Y14" s="50"/>
       <c r="Z14" s="50"/>
@@ -6248,35 +6260,35 @@
       <c r="AB14" s="50"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="49" t="s">
         <v>221</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="57" t="s">
+      <c r="B15" s="49"/>
+      <c r="C15" s="52" t="s">
         <v>220</v>
       </c>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
       <c r="J15" s="50"/>
       <c r="K15" s="50"/>
       <c r="L15" s="50"/>
       <c r="M15" s="50"/>
       <c r="N15" s="50"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
       <c r="Q15" s="50"/>
       <c r="R15" s="50"/>
       <c r="S15" s="50"/>
       <c r="T15" s="50"/>
       <c r="U15" s="50"/>
-      <c r="V15" s="49" t="s">
+      <c r="V15" s="51" t="s">
         <v>443</v>
       </c>
-      <c r="W15" s="49"/>
+      <c r="W15" s="51"/>
       <c r="X15" s="50" t="s">
         <v>442</v>
       </c>
@@ -6286,33 +6298,33 @@
       <c r="AB15" s="50"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="49" t="s">
         <v>222</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="57" t="s">
+      <c r="B16" s="49"/>
+      <c r="C16" s="52" t="s">
         <v>223</v>
       </c>
       <c r="D16" s="50"/>
       <c r="E16" s="50"/>
       <c r="F16" s="50"/>
       <c r="G16" s="50"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
       <c r="J16" s="50"/>
       <c r="K16" s="50"/>
       <c r="L16" s="50"/>
       <c r="M16" s="50"/>
       <c r="N16" s="50"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="49"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
       <c r="Q16" s="50"/>
       <c r="R16" s="50"/>
       <c r="S16" s="50"/>
       <c r="T16" s="50"/>
       <c r="U16" s="50"/>
-      <c r="V16" s="49"/>
-      <c r="W16" s="49"/>
+      <c r="V16" s="51"/>
+      <c r="W16" s="51"/>
       <c r="X16" s="50"/>
       <c r="Y16" s="50"/>
       <c r="Z16" s="50"/>
@@ -6320,10 +6332,10 @@
       <c r="AB16" s="50"/>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="49" t="s">
         <v>315</v>
       </c>
-      <c r="B17" s="53"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="50" t="s">
         <v>432</v>
       </c>
@@ -6331,22 +6343,22 @@
       <c r="E17" s="50"/>
       <c r="F17" s="50"/>
       <c r="G17" s="50"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="50"/>
       <c r="K17" s="50"/>
       <c r="L17" s="50"/>
       <c r="M17" s="50"/>
       <c r="N17" s="50"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="49"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
       <c r="Q17" s="50"/>
       <c r="R17" s="50"/>
       <c r="S17" s="50"/>
       <c r="T17" s="50"/>
       <c r="U17" s="50"/>
-      <c r="V17" s="49"/>
-      <c r="W17" s="49"/>
+      <c r="V17" s="51"/>
+      <c r="W17" s="51"/>
       <c r="X17" s="50"/>
       <c r="Y17" s="50"/>
       <c r="Z17" s="50"/>
@@ -6354,29 +6366,29 @@
       <c r="AB17" s="50"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="53"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="50"/>
       <c r="D18" s="50"/>
       <c r="E18" s="50"/>
       <c r="F18" s="50"/>
       <c r="G18" s="50"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
       <c r="L18" s="50"/>
       <c r="M18" s="50"/>
       <c r="N18" s="50"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
       <c r="Q18" s="50"/>
       <c r="R18" s="50"/>
       <c r="S18" s="50"/>
       <c r="T18" s="50"/>
       <c r="U18" s="50"/>
-      <c r="V18" s="49"/>
-      <c r="W18" s="49"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
       <c r="X18" s="50"/>
       <c r="Y18" s="50"/>
       <c r="Z18" s="50"/>
@@ -6384,29 +6396,29 @@
       <c r="AB18" s="50"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="50"/>
       <c r="D19" s="50"/>
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
       <c r="G19" s="50"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
       <c r="J19" s="50"/>
       <c r="K19" s="50"/>
       <c r="L19" s="50"/>
       <c r="M19" s="50"/>
       <c r="N19" s="50"/>
-      <c r="O19" s="49"/>
-      <c r="P19" s="49"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
       <c r="Q19" s="50"/>
       <c r="R19" s="50"/>
       <c r="S19" s="50"/>
       <c r="T19" s="50"/>
       <c r="U19" s="50"/>
-      <c r="V19" s="49"/>
-      <c r="W19" s="49"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="51"/>
       <c r="X19" s="50"/>
       <c r="Y19" s="50"/>
       <c r="Z19" s="50"/>
@@ -6414,29 +6426,29 @@
       <c r="AB19" s="50"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="50"/>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>
       <c r="F20" s="50"/>
       <c r="G20" s="50"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
       <c r="J20" s="50"/>
       <c r="K20" s="50"/>
       <c r="L20" s="50"/>
       <c r="M20" s="50"/>
       <c r="N20" s="50"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="49"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
       <c r="Q20" s="50"/>
       <c r="R20" s="50"/>
       <c r="S20" s="50"/>
       <c r="T20" s="50"/>
       <c r="U20" s="50"/>
-      <c r="V20" s="49"/>
-      <c r="W20" s="49"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
       <c r="X20" s="50"/>
       <c r="Y20" s="50"/>
       <c r="Z20" s="50"/>
@@ -6444,29 +6456,29 @@
       <c r="AB20" s="50"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="53"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="50"/>
       <c r="D21" s="50"/>
       <c r="E21" s="50"/>
       <c r="F21" s="50"/>
       <c r="G21" s="50"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
       <c r="J21" s="50"/>
       <c r="K21" s="50"/>
       <c r="L21" s="50"/>
       <c r="M21" s="50"/>
       <c r="N21" s="50"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="49"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
       <c r="Q21" s="50"/>
       <c r="R21" s="50"/>
       <c r="S21" s="50"/>
       <c r="T21" s="50"/>
       <c r="U21" s="50"/>
-      <c r="V21" s="49"/>
-      <c r="W21" s="49"/>
+      <c r="V21" s="51"/>
+      <c r="W21" s="51"/>
       <c r="X21" s="50"/>
       <c r="Y21" s="50"/>
       <c r="Z21" s="50"/>
@@ -6474,29 +6486,29 @@
       <c r="AB21" s="50"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="53"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="50"/>
       <c r="D22" s="50"/>
       <c r="E22" s="50"/>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
       <c r="J22" s="50"/>
       <c r="K22" s="50"/>
       <c r="L22" s="50"/>
       <c r="M22" s="50"/>
       <c r="N22" s="50"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
+      <c r="O22" s="51"/>
+      <c r="P22" s="51"/>
       <c r="Q22" s="50"/>
       <c r="R22" s="50"/>
       <c r="S22" s="50"/>
       <c r="T22" s="50"/>
       <c r="U22" s="50"/>
-      <c r="V22" s="49"/>
-      <c r="W22" s="49"/>
+      <c r="V22" s="51"/>
+      <c r="W22" s="51"/>
       <c r="X22" s="50"/>
       <c r="Y22" s="50"/>
       <c r="Z22" s="50"/>
@@ -6504,22 +6516,22 @@
       <c r="AB22" s="50"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="53"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
       <c r="E23" s="50"/>
       <c r="F23" s="50"/>
       <c r="G23" s="50"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
       <c r="J23" s="50"/>
       <c r="K23" s="50"/>
       <c r="L23" s="50"/>
       <c r="M23" s="50"/>
       <c r="N23" s="50"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="49"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
       <c r="Q23" s="50"/>
       <c r="R23" s="50"/>
       <c r="S23" s="50"/>
@@ -6527,22 +6539,22 @@
       <c r="U23" s="50"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="53"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="50"/>
       <c r="D24" s="50"/>
       <c r="E24" s="50"/>
       <c r="F24" s="50"/>
       <c r="G24" s="50"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
       <c r="J24" s="50"/>
       <c r="K24" s="50"/>
       <c r="L24" s="50"/>
       <c r="M24" s="50"/>
       <c r="N24" s="50"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="49"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
       <c r="Q24" s="50"/>
       <c r="R24" s="50"/>
       <c r="S24" s="50"/>
@@ -6550,22 +6562,22 @@
       <c r="U24" s="50"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="53"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
       <c r="E25" s="50"/>
       <c r="F25" s="50"/>
       <c r="G25" s="50"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
       <c r="J25" s="50"/>
       <c r="K25" s="50"/>
       <c r="L25" s="50"/>
       <c r="M25" s="50"/>
       <c r="N25" s="50"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="49"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
       <c r="Q25" s="50"/>
       <c r="R25" s="50"/>
       <c r="S25" s="50"/>
@@ -6573,22 +6585,22 @@
       <c r="U25" s="50"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
-      <c r="B26" s="53"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="50"/>
       <c r="D26" s="50"/>
       <c r="E26" s="50"/>
       <c r="F26" s="50"/>
       <c r="G26" s="50"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
       <c r="J26" s="50"/>
       <c r="K26" s="50"/>
       <c r="L26" s="50"/>
       <c r="M26" s="50"/>
       <c r="N26" s="50"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="49"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="51"/>
       <c r="Q26" s="50"/>
       <c r="R26" s="50"/>
       <c r="S26" s="50"/>
@@ -6596,22 +6608,22 @@
       <c r="U26" s="50"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
-      <c r="B27" s="53"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
       <c r="E27" s="50"/>
       <c r="F27" s="50"/>
       <c r="G27" s="50"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
       <c r="J27" s="50"/>
       <c r="K27" s="50"/>
       <c r="L27" s="50"/>
       <c r="M27" s="50"/>
       <c r="N27" s="50"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="49"/>
+      <c r="O27" s="51"/>
+      <c r="P27" s="51"/>
       <c r="Q27" s="50"/>
       <c r="R27" s="50"/>
       <c r="S27" s="50"/>
@@ -6619,22 +6631,22 @@
       <c r="U27" s="50"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
-      <c r="B28" s="53"/>
+      <c r="A28" s="49"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="50"/>
       <c r="D28" s="50"/>
       <c r="E28" s="50"/>
       <c r="F28" s="50"/>
       <c r="G28" s="50"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
       <c r="J28" s="50"/>
       <c r="K28" s="50"/>
       <c r="L28" s="50"/>
       <c r="M28" s="50"/>
       <c r="N28" s="50"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
       <c r="Q28" s="50"/>
       <c r="R28" s="50"/>
       <c r="S28" s="50"/>
@@ -6642,22 +6654,22 @@
       <c r="U28" s="50"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="53"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="50"/>
       <c r="D29" s="50"/>
       <c r="E29" s="50"/>
       <c r="F29" s="50"/>
       <c r="G29" s="50"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
       <c r="J29" s="50"/>
       <c r="K29" s="50"/>
       <c r="L29" s="50"/>
       <c r="M29" s="50"/>
       <c r="N29" s="50"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="51"/>
       <c r="Q29" s="50"/>
       <c r="R29" s="50"/>
       <c r="S29" s="50"/>
@@ -6665,22 +6677,22 @@
       <c r="U29" s="50"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
-      <c r="B30" s="53"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="50"/>
       <c r="D30" s="50"/>
       <c r="E30" s="50"/>
       <c r="F30" s="50"/>
       <c r="G30" s="50"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
       <c r="J30" s="50"/>
       <c r="K30" s="50"/>
       <c r="L30" s="50"/>
       <c r="M30" s="50"/>
       <c r="N30" s="50"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
       <c r="Q30" s="50"/>
       <c r="R30" s="50"/>
       <c r="S30" s="50"/>
@@ -6688,22 +6700,22 @@
       <c r="U30" s="50"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
-      <c r="B31" s="53"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="50"/>
       <c r="D31" s="50"/>
       <c r="E31" s="50"/>
       <c r="F31" s="50"/>
       <c r="G31" s="50"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
       <c r="J31" s="50"/>
       <c r="K31" s="50"/>
       <c r="L31" s="50"/>
       <c r="M31" s="50"/>
       <c r="N31" s="50"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
+      <c r="O31" s="51"/>
+      <c r="P31" s="51"/>
       <c r="Q31" s="50"/>
       <c r="R31" s="50"/>
       <c r="S31" s="50"/>
@@ -6711,22 +6723,22 @@
       <c r="U31" s="50"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="53"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="50"/>
       <c r="D32" s="50"/>
       <c r="E32" s="50"/>
       <c r="F32" s="50"/>
       <c r="G32" s="50"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
       <c r="J32" s="50"/>
       <c r="K32" s="50"/>
       <c r="L32" s="50"/>
       <c r="M32" s="50"/>
       <c r="N32" s="50"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
+      <c r="O32" s="51"/>
+      <c r="P32" s="51"/>
       <c r="Q32" s="50"/>
       <c r="R32" s="50"/>
       <c r="S32" s="50"/>
@@ -6734,22 +6746,22 @@
       <c r="U32" s="50"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
-      <c r="B33" s="53"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="50"/>
       <c r="D33" s="50"/>
       <c r="E33" s="50"/>
       <c r="F33" s="50"/>
       <c r="G33" s="50"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
       <c r="J33" s="50"/>
       <c r="K33" s="50"/>
       <c r="L33" s="50"/>
       <c r="M33" s="50"/>
       <c r="N33" s="50"/>
-      <c r="O33" s="53"/>
-      <c r="P33" s="53"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
       <c r="Q33" s="50"/>
       <c r="R33" s="50"/>
       <c r="S33" s="50"/>
@@ -6757,22 +6769,22 @@
       <c r="U33" s="50"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
-      <c r="B34" s="53"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="50"/>
       <c r="D34" s="50"/>
       <c r="E34" s="50"/>
       <c r="F34" s="50"/>
       <c r="G34" s="50"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
       <c r="J34" s="50"/>
       <c r="K34" s="50"/>
       <c r="L34" s="50"/>
       <c r="M34" s="50"/>
       <c r="N34" s="50"/>
-      <c r="O34" s="53"/>
-      <c r="P34" s="53"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
       <c r="Q34" s="50"/>
       <c r="R34" s="50"/>
       <c r="S34" s="50"/>
@@ -6780,8 +6792,8 @@
       <c r="U34" s="50"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
-      <c r="B35" s="53"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="50"/>
       <c r="D35" s="50"/>
       <c r="E35" s="50"/>
@@ -6790,141 +6802,85 @@
     </row>
   </sheetData>
   <mergeCells count="238">
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:U34"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:U33"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:U32"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:U31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:U30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:U29"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:U28"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:U26"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:U25"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:U24"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:U23"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="X22:AB22"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:AB21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:U21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:U22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="X20:AB20"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="X19:AB19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:U19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:U20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:AB18"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:AB17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:U17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:U18"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="X15:AB15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:U15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:U16"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="X14:AB14"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:AB5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:AB4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:N2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="V1:AB2"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="O1:U2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:AB7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:U10"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="X11:AB11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:U11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:G13"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="J16:N16"/>
     <mergeCell ref="V12:W12"/>
@@ -6949,85 +6905,141 @@
     <mergeCell ref="X16:AB16"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:G16"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:AB10"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:U10"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="X11:AB11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:U11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:AB8"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:AB7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:N2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="V1:AB2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="O1:U2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:AB5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:AB4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="X15:AB15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:U16"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="X14:AB14"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="X18:AB18"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:AB17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:U17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:U18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="X20:AB20"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="X19:AB19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:U19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:U20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="X22:AB22"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:AB21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:U21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:U22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:U24"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:U23"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:U26"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:U28"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:U30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:U29"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:U32"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:U31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:U34"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:U33"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:G33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C16" r:id="rId1" xr:uid="{868F8F85-B252-4B04-B081-E9B23AD46A23}"/>
@@ -7674,6 +7686,21 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="D20:G20"/>
@@ -7686,21 +7713,6 @@
     <mergeCell ref="D27:G27"/>
     <mergeCell ref="D28:G28"/>
     <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update game mechanics and weapon attributes
</commit_message>
<xml_diff>
--- a/plans/todo.xlsx
+++ b/plans/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edsquid\Documents\Personal Projects\Business\RogueLikeGame\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92E39BD-089C-4A49-8008-6676615AC18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA880ACB-438C-4276-8D9B-D2AFF4112406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30150" yWindow="1065" windowWidth="17415" windowHeight="13335" tabRatio="509" firstSheet="2" activeTab="4" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
+    <workbookView xWindow="30810" yWindow="885" windowWidth="17415" windowHeight="13335" tabRatio="509" firstSheet="2" activeTab="4" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="448">
   <si>
     <t>Max Lives</t>
   </si>
@@ -704,9 +704,6 @@
     <t>https://en.wikipedia.org/wiki/Kogarasu_Maru - Little crow circle</t>
   </si>
   <si>
-    <t>Little Crow Circle</t>
-  </si>
-  <si>
     <t>Sword Kladenets</t>
   </si>
   <si>
@@ -1383,13 +1380,19 @@
   </si>
   <si>
     <t>Sanctified Edge</t>
+  </si>
+  <si>
+    <t>Tui Camai</t>
+  </si>
+  <si>
+    <t>Magic Channel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1461,6 +1464,13 @@
       <b/>
       <sz val="22"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1702,7 +1712,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1802,13 +1812,13 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1820,10 +1830,19 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1844,8 +1863,11 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2560,7 +2582,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>61</v>
@@ -2778,7 +2800,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>97</v>
@@ -2814,7 +2836,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>97</v>
@@ -2865,13 +2887,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G41" s="2"/>
     </row>
@@ -2880,13 +2902,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G44" s="2"/>
     </row>
@@ -2924,7 +2946,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>63</v>
@@ -2945,7 +2967,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>63</v>
@@ -2984,7 +3006,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F54" s="1">
         <v>5</v>
@@ -3038,7 +3060,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3049,7 +3071,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>61</v>
@@ -3076,7 +3098,7 @@
         <v>61</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F67" s="1">
         <v>5</v>
@@ -3133,7 +3155,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G72" s="2"/>
     </row>
@@ -3157,7 +3179,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>65</v>
@@ -3205,7 +3227,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F81" s="1">
         <v>5</v>
@@ -3220,7 +3242,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>63</v>
@@ -3289,7 +3311,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F90" s="1">
         <v>5</v>
@@ -3316,7 +3338,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>65</v>
@@ -3328,7 +3350,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>65</v>
@@ -3347,7 +3369,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>65</v>
@@ -3365,7 +3387,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F99" s="1">
         <v>5</v>
@@ -3380,7 +3402,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F101" s="1">
         <v>5</v>
@@ -3620,13 +3642,13 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G133" s="2"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G134" s="2"/>
     </row>
@@ -3635,7 +3657,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G136" s="2"/>
     </row>
@@ -3763,7 +3785,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F158" s="1">
         <v>1</v>
@@ -3790,7 +3812,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F161" s="1">
         <v>1</v>
@@ -3805,7 +3827,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F163" s="1">
         <v>1</v>
@@ -3823,7 +3845,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F165" s="1">
         <v>1</v>
@@ -3859,7 +3881,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F169" s="1">
         <v>1</v>
@@ -3868,7 +3890,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F170" s="1">
         <v>1</v>
@@ -3904,7 +3926,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F175" s="1">
         <v>5</v>
@@ -3964,7 +3986,7 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F183" s="1">
         <v>5</v>
@@ -4087,7 +4109,7 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="42" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B200" s="42"/>
       <c r="C200" s="42"/>
@@ -4098,7 +4120,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F201" s="1">
         <v>5</v>
@@ -4107,7 +4129,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F202" s="1">
         <v>5</v>
@@ -4116,7 +4138,7 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F203" s="1">
         <v>5</v>
@@ -4125,7 +4147,7 @@
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F204" s="1">
         <v>5</v>
@@ -4134,7 +4156,7 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F205" s="1">
         <v>5</v>
@@ -4152,7 +4174,7 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F207" s="1">
         <v>5</v>
@@ -4176,7 +4198,7 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F210" s="1">
         <v>5</v>
@@ -4209,7 +4231,7 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F214" s="1">
         <v>5</v>
@@ -4236,7 +4258,7 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="23" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F218" s="1">
         <v>5</v>
@@ -4245,7 +4267,7 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F219" s="1">
         <v>5</v>
@@ -4254,7 +4276,7 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F220" s="1">
         <v>5</v>
@@ -4263,7 +4285,7 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F221" s="1">
         <v>5</v>
@@ -4272,7 +4294,7 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F222" s="1">
         <v>5</v>
@@ -4290,7 +4312,7 @@
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F224" s="1">
         <v>5</v>
@@ -4299,7 +4321,7 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F225" s="1">
         <v>5</v>
@@ -4317,7 +4339,7 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F227" s="1">
         <v>5</v>
@@ -4335,7 +4357,7 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F229" s="1">
         <v>5</v>
@@ -4353,7 +4375,7 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F231" s="1">
         <v>5</v>
@@ -4371,7 +4393,7 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F233" s="1">
         <v>5</v>
@@ -4386,7 +4408,7 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F235" s="1">
         <v>5</v>
@@ -4395,7 +4417,7 @@
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F236" s="1">
         <v>5</v>
@@ -4404,7 +4426,7 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F237" s="1">
         <v>5</v>
@@ -4413,7 +4435,7 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F238" s="1">
         <v>5</v>
@@ -4422,7 +4444,7 @@
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F239" s="1">
         <v>5</v>
@@ -4440,7 +4462,7 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F241" s="1">
         <v>5</v>
@@ -4458,7 +4480,7 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>61</v>
@@ -4476,7 +4498,7 @@
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F244" s="1">
         <v>5</v>
@@ -4490,12 +4512,12 @@
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F247" s="1">
         <v>5</v>
@@ -4513,7 +4535,7 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F249" s="1">
         <v>5</v>
@@ -4540,7 +4562,7 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F253" s="1">
         <v>5</v>
@@ -4549,7 +4571,7 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F254" s="1">
         <v>5</v>
@@ -4558,7 +4580,7 @@
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F255" s="1">
         <v>5</v>
@@ -4567,7 +4589,7 @@
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F256" s="1">
         <v>5</v>
@@ -4576,7 +4598,7 @@
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F257" s="1">
         <v>5</v>
@@ -4594,7 +4616,7 @@
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F259" s="1">
         <v>5</v>
@@ -4603,7 +4625,7 @@
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F260" s="1">
         <v>5</v>
@@ -4619,7 +4641,7 @@
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F262" s="1">
         <v>5</v>
@@ -4637,7 +4659,7 @@
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F264" s="1">
         <v>5</v>
@@ -4655,7 +4677,7 @@
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F266" s="1">
         <v>5</v>
@@ -4676,7 +4698,7 @@
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F269" s="1">
         <v>5</v>
@@ -4685,7 +4707,7 @@
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F270" s="1">
         <v>5</v>
@@ -4694,7 +4716,7 @@
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F271" s="1">
         <v>5</v>
@@ -4703,7 +4725,7 @@
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F272" s="1">
         <v>5</v>
@@ -4712,7 +4734,7 @@
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F273" s="1">
         <v>5</v>
@@ -4760,7 +4782,7 @@
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F279" s="1">
         <v>5</v>
@@ -4778,7 +4800,7 @@
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F281" s="1">
         <v>5</v>
@@ -4805,7 +4827,7 @@
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" s="29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F285" s="1">
         <v>5</v>
@@ -4814,7 +4836,7 @@
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F286" s="1">
         <v>5</v>
@@ -4823,7 +4845,7 @@
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F287" s="1">
         <v>5</v>
@@ -4832,7 +4854,7 @@
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F288" s="1">
         <v>5</v>
@@ -4841,7 +4863,7 @@
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F289" s="1">
         <v>5</v>
@@ -4859,7 +4881,7 @@
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F291" s="1">
         <v>5</v>
@@ -4868,7 +4890,7 @@
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F292" s="1">
         <v>5</v>
@@ -4886,7 +4908,7 @@
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F294" s="1">
         <v>5</v>
@@ -4895,7 +4917,7 @@
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F295" s="1">
         <v>5</v>
@@ -4913,7 +4935,7 @@
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F297" s="1">
         <v>5</v>
@@ -4937,7 +4959,7 @@
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F300" s="1">
         <v>5</v>
@@ -5544,7 +5566,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -5582,7 +5604,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B4" s="47"/>
       <c r="C4" s="47"/>
@@ -5596,47 +5618,47 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -5653,8 +5675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E13E4A5-10AD-4171-99FD-31881C0A6C11}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5789,22 +5811,22 @@
       <c r="AA3" s="56"/>
       <c r="AB3" s="56"/>
     </row>
-    <row r="4" spans="1:30" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+    <row r="4" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>344</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="52" t="s">
         <v>345</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="51" t="s">
-        <v>346</v>
-      </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52" t="s">
-        <v>297</v>
-      </c>
-      <c r="I4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="53" t="s">
+        <v>296</v>
+      </c>
+      <c r="I4" s="53"/>
       <c r="J4" s="50" t="s">
         <v>35</v>
       </c>
@@ -5812,10 +5834,10 @@
       <c r="L4" s="50"/>
       <c r="M4" s="50"/>
       <c r="N4" s="50"/>
-      <c r="O4" s="49" t="s">
-        <v>308</v>
-      </c>
-      <c r="P4" s="49"/>
+      <c r="O4" s="57" t="s">
+        <v>307</v>
+      </c>
+      <c r="P4" s="57"/>
       <c r="Q4" s="50" t="s">
         <v>150</v>
       </c>
@@ -5835,11 +5857,11 @@
       <c r="AA4" s="50"/>
       <c r="AB4" s="50"/>
     </row>
-    <row r="5" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
-        <v>344</v>
-      </c>
-      <c r="B5" s="52"/>
+    <row r="5" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
+        <v>343</v>
+      </c>
+      <c r="B5" s="53"/>
       <c r="C5" s="50" t="s">
         <v>34</v>
       </c>
@@ -5847,23 +5869,23 @@
       <c r="E5" s="50"/>
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
-      <c r="H5" s="52" t="s">
+      <c r="H5" s="53" t="s">
+        <v>297</v>
+      </c>
+      <c r="I5" s="53"/>
+      <c r="J5" s="50" t="s">
         <v>298</v>
-      </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="50" t="s">
-        <v>299</v>
       </c>
       <c r="K5" s="50"/>
       <c r="L5" s="50"/>
       <c r="M5" s="50"/>
       <c r="N5" s="50"/>
-      <c r="O5" s="49" t="s">
+      <c r="O5" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="P5" s="49"/>
+      <c r="P5" s="57"/>
       <c r="Q5" s="50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R5" s="50"/>
       <c r="S5" s="50"/>
@@ -5881,11 +5903,11 @@
       <c r="AA5" s="50"/>
       <c r="AB5" s="50"/>
     </row>
-    <row r="6" spans="1:30" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
-        <v>347</v>
-      </c>
-      <c r="B6" s="52"/>
+    <row r="6" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
+        <v>346</v>
+      </c>
+      <c r="B6" s="53"/>
       <c r="C6" s="50" t="s">
         <v>212</v>
       </c>
@@ -5893,10 +5915,10 @@
       <c r="E6" s="50"/>
       <c r="F6" s="50"/>
       <c r="G6" s="50"/>
-      <c r="H6" s="52" t="s">
-        <v>300</v>
-      </c>
-      <c r="I6" s="52"/>
+      <c r="H6" s="53" t="s">
+        <v>299</v>
+      </c>
+      <c r="I6" s="53"/>
       <c r="J6" s="50" t="s">
         <v>37</v>
       </c>
@@ -5904,12 +5926,12 @@
       <c r="L6" s="50"/>
       <c r="M6" s="50"/>
       <c r="N6" s="50"/>
-      <c r="O6" s="49" t="s">
+      <c r="O6" s="57" t="s">
         <v>152</v>
       </c>
-      <c r="P6" s="49"/>
+      <c r="P6" s="57"/>
       <c r="Q6" s="50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R6" s="50"/>
       <c r="S6" s="50"/>
@@ -5923,9 +5945,9 @@
       <c r="AA6" s="50"/>
       <c r="AB6" s="50"/>
     </row>
-    <row r="7" spans="1:30" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B7" s="53"/>
       <c r="C7" s="50" t="s">
@@ -5935,30 +5957,30 @@
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
-      <c r="H7" s="57" t="s">
-        <v>307</v>
-      </c>
-      <c r="I7" s="57"/>
+      <c r="H7" s="58" t="s">
+        <v>306</v>
+      </c>
+      <c r="I7" s="58"/>
       <c r="J7" s="50" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K7" s="50"/>
       <c r="L7" s="50"/>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
-      <c r="O7" s="49" t="s">
+      <c r="O7" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="P7" s="49"/>
+      <c r="P7" s="57"/>
       <c r="Q7" s="50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R7" s="50"/>
       <c r="S7" s="50"/>
       <c r="T7" s="50"/>
       <c r="U7" s="50"/>
       <c r="V7" s="49" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="W7" s="49"/>
       <c r="X7" s="50" t="s">
@@ -5969,31 +5991,31 @@
       <c r="AA7" s="50"/>
       <c r="AB7" s="50"/>
     </row>
-    <row r="8" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="53"/>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
       <c r="J8" s="50"/>
       <c r="K8" s="50"/>
       <c r="L8" s="50"/>
       <c r="M8" s="50"/>
       <c r="N8" s="50"/>
-      <c r="O8" s="49" t="s">
-        <v>313</v>
-      </c>
-      <c r="P8" s="49"/>
+      <c r="O8" s="57" t="s">
+        <v>312</v>
+      </c>
+      <c r="P8" s="57"/>
       <c r="Q8" s="50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R8" s="50"/>
       <c r="S8" s="50"/>
@@ -6011,40 +6033,40 @@
       <c r="AA8" s="50"/>
       <c r="AB8" s="50"/>
     </row>
-    <row r="9" spans="1:30" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B9" s="53"/>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="57" t="s">
         <v>211</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="52" t="s">
-        <v>306</v>
-      </c>
-      <c r="I9" s="52"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="53" t="s">
+        <v>305</v>
+      </c>
+      <c r="I9" s="53"/>
       <c r="J9" s="50" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K9" s="50"/>
       <c r="L9" s="50"/>
       <c r="M9" s="50"/>
       <c r="N9" s="50"/>
-      <c r="O9" s="49" t="s">
-        <v>302</v>
-      </c>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="50" t="s">
-        <v>267</v>
-      </c>
-      <c r="R9" s="50"/>
-      <c r="S9" s="50"/>
-      <c r="T9" s="50"/>
-      <c r="U9" s="50"/>
+      <c r="O9" s="57" t="s">
+        <v>301</v>
+      </c>
+      <c r="P9" s="57"/>
+      <c r="Q9" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="R9" s="57"/>
+      <c r="S9" s="57"/>
+      <c r="T9" s="57"/>
+      <c r="U9" s="57"/>
       <c r="V9" s="49" t="s">
         <v>47</v>
       </c>
@@ -6057,31 +6079,35 @@
       <c r="AA9" s="50"/>
       <c r="AB9" s="50"/>
     </row>
-    <row r="10" spans="1:30" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
+    <row r="10" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
+        <v>32</v>
+      </c>
       <c r="B10" s="53"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="52" t="s">
+      <c r="C10" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="53" t="s">
+        <v>431</v>
+      </c>
+      <c r="I10" s="53"/>
+      <c r="J10" s="50" t="s">
         <v>432</v>
-      </c>
-      <c r="I10" s="52"/>
-      <c r="J10" s="50" t="s">
-        <v>433</v>
       </c>
       <c r="K10" s="50"/>
       <c r="L10" s="50"/>
       <c r="M10" s="50"/>
       <c r="N10" s="50"/>
       <c r="O10" s="49" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="P10" s="49"/>
       <c r="Q10" s="50" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="R10" s="50"/>
       <c r="S10" s="50"/>
@@ -6099,22 +6125,22 @@
       <c r="AA10" s="50"/>
       <c r="AB10" s="50"/>
     </row>
-    <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
-        <v>32</v>
+        <v>217</v>
       </c>
       <c r="B11" s="53"/>
-      <c r="C11" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="I11" s="57"/>
+      <c r="C11" s="61" t="s">
+        <v>216</v>
+      </c>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="58" t="s">
+        <v>304</v>
+      </c>
+      <c r="I11" s="58"/>
       <c r="J11" s="50" t="s">
         <v>40</v>
       </c>
@@ -6123,11 +6149,11 @@
       <c r="M11" s="50"/>
       <c r="N11" s="50"/>
       <c r="O11" s="49" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P11" s="49"/>
       <c r="Q11" s="50" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="R11" s="50"/>
       <c r="S11" s="50"/>
@@ -6138,25 +6164,29 @@
       </c>
       <c r="W11" s="49"/>
       <c r="X11" s="50" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Y11" s="50"/>
       <c r="Z11" s="50"/>
       <c r="AA11" s="50"/>
       <c r="AB11" s="50"/>
     </row>
-    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+    <row r="12" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
+        <v>446</v>
+      </c>
       <c r="B12" s="53"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="52" t="s">
-        <v>304</v>
-      </c>
-      <c r="I12" s="52"/>
+      <c r="C12" s="60" t="s">
+        <v>219</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="53" t="s">
+        <v>303</v>
+      </c>
+      <c r="I12" s="53"/>
       <c r="J12" s="50" t="s">
         <v>210</v>
       </c>
@@ -6164,33 +6194,43 @@
       <c r="L12" s="50"/>
       <c r="M12" s="50"/>
       <c r="N12" s="50"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="49"/>
+      <c r="O12" s="57" t="s">
+        <v>435</v>
+      </c>
+      <c r="P12" s="57"/>
       <c r="Q12" s="50"/>
       <c r="R12" s="50"/>
       <c r="S12" s="50"/>
       <c r="T12" s="50"/>
       <c r="U12" s="50"/>
-      <c r="V12" s="49"/>
-      <c r="W12" s="49"/>
-      <c r="X12" s="50"/>
+      <c r="V12" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="W12" s="59"/>
+      <c r="X12" s="50" t="s">
+        <v>45</v>
+      </c>
       <c r="Y12" s="50"/>
       <c r="Z12" s="50"/>
       <c r="AA12" s="50"/>
       <c r="AB12" s="50"/>
     </row>
-    <row r="13" spans="1:30" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
+    <row r="13" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="53" t="s">
+        <v>220</v>
+      </c>
       <c r="B13" s="53"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="52" t="s">
-        <v>310</v>
-      </c>
-      <c r="I13" s="52"/>
+      <c r="C13" s="60" t="s">
+        <v>221</v>
+      </c>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="53" t="s">
+        <v>309</v>
+      </c>
+      <c r="I13" s="53"/>
       <c r="J13" s="50" t="s">
         <v>36</v>
       </c>
@@ -6198,81 +6238,69 @@
       <c r="L13" s="50"/>
       <c r="M13" s="50"/>
       <c r="N13" s="50"/>
-      <c r="O13" s="49" t="s">
-        <v>303</v>
-      </c>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="50" t="s">
+      <c r="O13" s="68" t="s">
+        <v>302</v>
+      </c>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="R13" s="50"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="50"/>
-      <c r="V13" s="53" t="s">
-        <v>218</v>
-      </c>
-      <c r="W13" s="53"/>
-      <c r="X13" s="50" t="s">
-        <v>45</v>
-      </c>
+      <c r="R13" s="69"/>
+      <c r="S13" s="69"/>
+      <c r="T13" s="69"/>
+      <c r="U13" s="69"/>
+      <c r="V13" s="49" t="s">
+        <v>437</v>
+      </c>
+      <c r="W13" s="49"/>
+      <c r="X13" s="50"/>
       <c r="Y13" s="50"/>
       <c r="Z13" s="50"/>
       <c r="AA13" s="50"/>
       <c r="AB13" s="50"/>
     </row>
-    <row r="14" spans="1:30" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="53" t="s">
-        <v>217</v>
+        <v>313</v>
       </c>
       <c r="B14" s="53"/>
-      <c r="C14" s="58" t="s">
-        <v>216</v>
-      </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
+      <c r="C14" s="50" t="s">
+        <v>430</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
       <c r="L14" s="50"/>
       <c r="M14" s="50"/>
       <c r="N14" s="50"/>
-      <c r="O14" s="49" t="s">
-        <v>436</v>
-      </c>
-      <c r="P14" s="49"/>
+      <c r="O14" s="17" t="s">
+        <v>447</v>
+      </c>
       <c r="Q14" s="50"/>
       <c r="R14" s="50"/>
       <c r="S14" s="50"/>
       <c r="T14" s="50"/>
       <c r="U14" s="50"/>
       <c r="V14" s="49" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="W14" s="49"/>
-      <c r="X14" s="50"/>
+      <c r="X14" s="50" t="s">
+        <v>440</v>
+      </c>
       <c r="Y14" s="50"/>
       <c r="Z14" s="50"/>
       <c r="AA14" s="50"/>
       <c r="AB14" s="50"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
-        <v>220</v>
-      </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="58" t="s">
-        <v>219</v>
-      </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
+    <row r="15" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
       <c r="J15" s="50"/>
       <c r="K15" s="50"/>
       <c r="L15" s="50"/>
@@ -6285,32 +6313,10 @@
       <c r="S15" s="50"/>
       <c r="T15" s="50"/>
       <c r="U15" s="50"/>
-      <c r="V15" s="49" t="s">
-        <v>442</v>
-      </c>
-      <c r="W15" s="49"/>
-      <c r="X15" s="50" t="s">
-        <v>441</v>
-      </c>
-      <c r="Y15" s="50"/>
-      <c r="Z15" s="50"/>
-      <c r="AA15" s="50"/>
-      <c r="AB15" s="50"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
-        <v>221</v>
-      </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="58" t="s">
-        <v>222</v>
-      </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
+    </row>
+    <row r="16" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
       <c r="J16" s="50"/>
       <c r="K16" s="50"/>
       <c r="L16" s="50"/>
@@ -6331,20 +6337,9 @@
       <c r="AA16" s="50"/>
       <c r="AB16" s="50"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
-        <v>314</v>
-      </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="50" t="s">
-        <v>431</v>
-      </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
+    <row r="17" spans="1:28" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
       <c r="J17" s="50"/>
       <c r="K17" s="50"/>
       <c r="L17" s="50"/>
@@ -6365,16 +6360,16 @@
       <c r="AA17" s="50"/>
       <c r="AB17" s="50"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="53"/>
+    <row r="18" spans="1:28" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="59"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="50"/>
       <c r="D18" s="50"/>
       <c r="E18" s="50"/>
       <c r="F18" s="50"/>
       <c r="G18" s="50"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
       <c r="L18" s="50"/>
@@ -6396,15 +6391,15 @@
       <c r="AB18" s="50"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="50"/>
       <c r="D19" s="50"/>
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
       <c r="G19" s="50"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
       <c r="J19" s="50"/>
       <c r="K19" s="50"/>
       <c r="L19" s="50"/>
@@ -6426,15 +6421,15 @@
       <c r="AB19" s="50"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
+      <c r="A20" s="59"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="50"/>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>
       <c r="F20" s="50"/>
       <c r="G20" s="50"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
       <c r="J20" s="50"/>
       <c r="K20" s="50"/>
       <c r="L20" s="50"/>
@@ -6456,15 +6451,15 @@
       <c r="AB20" s="50"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="53"/>
+      <c r="A21" s="59"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="50"/>
       <c r="D21" s="50"/>
       <c r="E21" s="50"/>
       <c r="F21" s="50"/>
       <c r="G21" s="50"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
       <c r="J21" s="50"/>
       <c r="K21" s="50"/>
       <c r="L21" s="50"/>
@@ -6486,15 +6481,15 @@
       <c r="AB21" s="50"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="53"/>
+      <c r="A22" s="59"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="50"/>
       <c r="D22" s="50"/>
       <c r="E22" s="50"/>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
       <c r="J22" s="50"/>
       <c r="K22" s="50"/>
       <c r="L22" s="50"/>
@@ -6516,15 +6511,15 @@
       <c r="AB22" s="50"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="53"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="59"/>
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
       <c r="E23" s="50"/>
       <c r="F23" s="50"/>
       <c r="G23" s="50"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
       <c r="J23" s="50"/>
       <c r="K23" s="50"/>
       <c r="L23" s="50"/>
@@ -6539,15 +6534,15 @@
       <c r="U23" s="50"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="53"/>
+      <c r="A24" s="59"/>
+      <c r="B24" s="59"/>
       <c r="C24" s="50"/>
       <c r="D24" s="50"/>
       <c r="E24" s="50"/>
       <c r="F24" s="50"/>
       <c r="G24" s="50"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
       <c r="J24" s="50"/>
       <c r="K24" s="50"/>
       <c r="L24" s="50"/>
@@ -6562,15 +6557,15 @@
       <c r="U24" s="50"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="53"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
       <c r="E25" s="50"/>
       <c r="F25" s="50"/>
       <c r="G25" s="50"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
       <c r="J25" s="50"/>
       <c r="K25" s="50"/>
       <c r="L25" s="50"/>
@@ -6585,15 +6580,15 @@
       <c r="U25" s="50"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
-      <c r="B26" s="53"/>
+      <c r="A26" s="59"/>
+      <c r="B26" s="59"/>
       <c r="C26" s="50"/>
       <c r="D26" s="50"/>
       <c r="E26" s="50"/>
       <c r="F26" s="50"/>
       <c r="G26" s="50"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
       <c r="J26" s="50"/>
       <c r="K26" s="50"/>
       <c r="L26" s="50"/>
@@ -6608,15 +6603,15 @@
       <c r="U26" s="50"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
-      <c r="B27" s="53"/>
+      <c r="A27" s="59"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
       <c r="E27" s="50"/>
       <c r="F27" s="50"/>
       <c r="G27" s="50"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="59"/>
       <c r="J27" s="50"/>
       <c r="K27" s="50"/>
       <c r="L27" s="50"/>
@@ -6631,15 +6626,15 @@
       <c r="U27" s="50"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
-      <c r="B28" s="53"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="59"/>
       <c r="C28" s="50"/>
       <c r="D28" s="50"/>
       <c r="E28" s="50"/>
       <c r="F28" s="50"/>
       <c r="G28" s="50"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
       <c r="J28" s="50"/>
       <c r="K28" s="50"/>
       <c r="L28" s="50"/>
@@ -6654,15 +6649,15 @@
       <c r="U28" s="50"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="53"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="59"/>
       <c r="C29" s="50"/>
       <c r="D29" s="50"/>
       <c r="E29" s="50"/>
       <c r="F29" s="50"/>
       <c r="G29" s="50"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
       <c r="J29" s="50"/>
       <c r="K29" s="50"/>
       <c r="L29" s="50"/>
@@ -6677,15 +6672,15 @@
       <c r="U29" s="50"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
-      <c r="B30" s="53"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="50"/>
       <c r="D30" s="50"/>
       <c r="E30" s="50"/>
       <c r="F30" s="50"/>
       <c r="G30" s="50"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="59"/>
       <c r="J30" s="50"/>
       <c r="K30" s="50"/>
       <c r="L30" s="50"/>
@@ -6700,15 +6695,15 @@
       <c r="U30" s="50"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
-      <c r="B31" s="53"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="50"/>
       <c r="D31" s="50"/>
       <c r="E31" s="50"/>
       <c r="F31" s="50"/>
       <c r="G31" s="50"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="59"/>
       <c r="J31" s="50"/>
       <c r="K31" s="50"/>
       <c r="L31" s="50"/>
@@ -6723,15 +6718,15 @@
       <c r="U31" s="50"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="53"/>
+      <c r="A32" s="59"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="50"/>
       <c r="D32" s="50"/>
       <c r="E32" s="50"/>
       <c r="F32" s="50"/>
       <c r="G32" s="50"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="59"/>
       <c r="J32" s="50"/>
       <c r="K32" s="50"/>
       <c r="L32" s="50"/>
@@ -6746,22 +6741,22 @@
       <c r="U32" s="50"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
-      <c r="B33" s="53"/>
+      <c r="A33" s="59"/>
+      <c r="B33" s="59"/>
       <c r="C33" s="50"/>
       <c r="D33" s="50"/>
       <c r="E33" s="50"/>
       <c r="F33" s="50"/>
       <c r="G33" s="50"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
       <c r="J33" s="50"/>
       <c r="K33" s="50"/>
       <c r="L33" s="50"/>
       <c r="M33" s="50"/>
       <c r="N33" s="50"/>
-      <c r="O33" s="53"/>
-      <c r="P33" s="53"/>
+      <c r="O33" s="59"/>
+      <c r="P33" s="59"/>
       <c r="Q33" s="50"/>
       <c r="R33" s="50"/>
       <c r="S33" s="50"/>
@@ -6769,22 +6764,22 @@
       <c r="U33" s="50"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
-      <c r="B34" s="53"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="59"/>
       <c r="C34" s="50"/>
       <c r="D34" s="50"/>
       <c r="E34" s="50"/>
       <c r="F34" s="50"/>
       <c r="G34" s="50"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="59"/>
       <c r="J34" s="50"/>
       <c r="K34" s="50"/>
       <c r="L34" s="50"/>
       <c r="M34" s="50"/>
       <c r="N34" s="50"/>
-      <c r="O34" s="53"/>
-      <c r="P34" s="53"/>
+      <c r="O34" s="59"/>
+      <c r="P34" s="59"/>
       <c r="Q34" s="50"/>
       <c r="R34" s="50"/>
       <c r="S34" s="50"/>
@@ -6792,8 +6787,8 @@
       <c r="U34" s="50"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
-      <c r="B35" s="53"/>
+      <c r="A35" s="59"/>
+      <c r="B35" s="59"/>
       <c r="C35" s="50"/>
       <c r="D35" s="50"/>
       <c r="E35" s="50"/>
@@ -6801,7 +6796,7 @@
       <c r="G35" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="238">
+  <mergeCells count="229">
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="H34:I34"/>
@@ -6922,56 +6917,47 @@
     <mergeCell ref="Q18:U18"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="J17:N17"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="X15:AB15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="X14:AB14"/>
     <mergeCell ref="O15:P15"/>
     <mergeCell ref="Q15:U15"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="Q16:U16"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="J14:N14"/>
     <mergeCell ref="V13:W13"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="X14:AB14"/>
+    <mergeCell ref="X13:AB13"/>
     <mergeCell ref="Q14:U14"/>
     <mergeCell ref="V16:W16"/>
-    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="H14:I14"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="J16:N16"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="X12:AB12"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:G12"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="J15:N15"/>
-    <mergeCell ref="O12:P12"/>
     <mergeCell ref="Q12:U12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="J12:N12"/>
     <mergeCell ref="O13:P13"/>
     <mergeCell ref="Q13:U13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="J13:N13"/>
-    <mergeCell ref="X13:AB13"/>
+    <mergeCell ref="X12:AB12"/>
     <mergeCell ref="X16:AB16"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:AB10"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:G13"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:N9"/>
     <mergeCell ref="V9:W9"/>
@@ -7042,9 +7028,9 @@
     <mergeCell ref="J5:N5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C16" r:id="rId1" xr:uid="{868F8F85-B252-4B04-B081-E9B23AD46A23}"/>
-    <hyperlink ref="C15" r:id="rId2" xr:uid="{86E514BE-A9C9-4B5A-AB4D-57536B7FEAAB}"/>
-    <hyperlink ref="C14" r:id="rId3" xr:uid="{CE321704-25F7-4D6A-8585-A2ECF5644FEF}"/>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{868F8F85-B252-4B04-B081-E9B23AD46A23}"/>
+    <hyperlink ref="C12" r:id="rId2" xr:uid="{86E514BE-A9C9-4B5A-AB4D-57536B7FEAAB}"/>
+    <hyperlink ref="C11" r:id="rId3" xr:uid="{CE321704-25F7-4D6A-8585-A2ECF5644FEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -7074,128 +7060,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
+      <c r="A1" s="64" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="D2" s="33" t="s">
+      <c r="E2" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E2" s="33" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="3" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="62" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C4" s="35">
         <v>2</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>244</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>245</v>
       </c>
       <c r="C5" s="35">
         <v>3</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C6" s="35">
         <v>1</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" s="34" t="s">
         <v>269</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>270</v>
       </c>
       <c r="C7" s="35">
         <v>2</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="35">
         <v>1</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9" s="34" t="s">
         <v>14</v>
@@ -7204,16 +7190,16 @@
         <v>2</v>
       </c>
       <c r="D9" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="E9" s="35" t="s">
         <v>240</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>14</v>
@@ -7222,110 +7208,110 @@
         <v>4</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
+        <v>420</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>421</v>
       </c>
-      <c r="B13" s="36" t="s">
-        <v>422</v>
-      </c>
       <c r="C13" s="37">
         <v>5</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="59" t="s">
-        <v>429</v>
-      </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
+      <c r="A19" s="62" t="s">
+        <v>428</v>
+      </c>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>231</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>232</v>
       </c>
       <c r="C21" s="32">
         <v>1</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>419</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>420</v>
       </c>
       <c r="C22" s="32">
         <v>2</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E23" s="32"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E24" s="32"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>430</v>
-      </c>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
+        <v>429</v>
+      </c>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -7364,15 +7350,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="63" t="s">
-        <v>248</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
+      <c r="A1" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -7382,307 +7368,307 @@
         <v>181</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="D2" s="64" t="s">
-        <v>229</v>
-      </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
+        <v>225</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
       <c r="I2" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" s="65" t="s">
         <v>249</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="62" t="s">
-        <v>250</v>
-      </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
       <c r="I3" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>257</v>
-      </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
+        <v>229</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>256</v>
+      </c>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
       <c r="J4" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" s="65" t="s">
         <v>253</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="D5" s="62" t="s">
-        <v>254</v>
-      </c>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
       <c r="J5" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D6" s="62" t="s">
-        <v>251</v>
-      </c>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
+        <v>255</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>250</v>
+      </c>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
+        <v>280</v>
+      </c>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
       <c r="I10" s="5" t="s">
         <v>156</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D11" s="65" t="s">
         <v>286</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="D11" s="62" t="s">
-        <v>287</v>
-      </c>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
       <c r="J11" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="65" t="s">
         <v>262</v>
       </c>
-      <c r="D12" s="62" t="s">
-        <v>263</v>
-      </c>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
       <c r="I12" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="J12" s="14" t="s">
         <v>291</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="65" t="s">
         <v>265</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="D13" s="62" t="s">
-        <v>266</v>
-      </c>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="65" t="s">
         <v>295</v>
       </c>
-      <c r="D14" s="62" t="s">
-        <v>296</v>
-      </c>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
     </row>
     <row r="17" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D17" s="63" t="s">
         <v>276</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="D17" s="60" t="s">
-        <v>277</v>
-      </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="27">

</xml_diff>

<commit_message>
Update weapon and sprite animations
</commit_message>
<xml_diff>
--- a/plans/todo.xlsx
+++ b/plans/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edsquid\Documents\Personal Projects\Business\RogueLikeGame\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA880ACB-438C-4276-8D9B-D2AFF4112406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0854B78F-6C09-41A6-99D5-D8C3E3A58CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30810" yWindow="885" windowWidth="17415" windowHeight="13335" tabRatio="509" firstSheet="2" activeTab="4" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
+    <workbookView xWindow="32580" yWindow="780" windowWidth="17415" windowHeight="13335" tabRatio="509" firstSheet="2" activeTab="4" xr2:uid="{BA1E511D-BF64-4842-98DF-72E30276ED1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="3" r:id="rId1"/>
@@ -1807,18 +1807,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1830,20 +1845,11 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1862,12 +1868,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5675,8 +5675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E13E4A5-10AD-4171-99FD-31881C0A6C11}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7:P7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7:AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5695,138 +5695,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54" t="s">
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59" t="s">
         <v>149</v>
       </c>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54" t="s">
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
       <c r="AD1" s="18" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="60"/>
+      <c r="C3" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="55" t="s">
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="55"/>
-      <c r="J3" s="56" t="s">
+      <c r="I3" s="60"/>
+      <c r="J3" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="55" t="s">
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="56" t="s">
+      <c r="P3" s="60"/>
+      <c r="Q3" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="55" t="s">
+      <c r="R3" s="61"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="V3" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="55"/>
-      <c r="X3" s="56" t="s">
+      <c r="W3" s="60"/>
+      <c r="X3" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="56"/>
+      <c r="Y3" s="61"/>
+      <c r="Z3" s="61"/>
+      <c r="AA3" s="61"/>
+      <c r="AB3" s="61"/>
     </row>
     <row r="4" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="62" t="s">
         <v>344</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="62"/>
+      <c r="C4" s="63" t="s">
         <v>345</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="53" t="s">
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="52" t="s">
         <v>296</v>
       </c>
-      <c r="I4" s="53"/>
+      <c r="I4" s="52"/>
       <c r="J4" s="50" t="s">
         <v>35</v>
       </c>
@@ -5834,10 +5834,10 @@
       <c r="L4" s="50"/>
       <c r="M4" s="50"/>
       <c r="N4" s="50"/>
-      <c r="O4" s="57" t="s">
+      <c r="O4" s="54" t="s">
         <v>307</v>
       </c>
-      <c r="P4" s="57"/>
+      <c r="P4" s="54"/>
       <c r="Q4" s="50" t="s">
         <v>150</v>
       </c>
@@ -5845,10 +5845,10 @@
       <c r="S4" s="50"/>
       <c r="T4" s="50"/>
       <c r="U4" s="50"/>
-      <c r="V4" s="49" t="s">
+      <c r="V4" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="W4" s="49"/>
+      <c r="W4" s="51"/>
       <c r="X4" s="50" t="s">
         <v>41</v>
       </c>
@@ -5858,10 +5858,10 @@
       <c r="AB4" s="50"/>
     </row>
     <row r="5" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="52" t="s">
         <v>343</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="50" t="s">
         <v>34</v>
       </c>
@@ -5869,10 +5869,10 @@
       <c r="E5" s="50"/>
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="52" t="s">
         <v>297</v>
       </c>
-      <c r="I5" s="53"/>
+      <c r="I5" s="52"/>
       <c r="J5" s="50" t="s">
         <v>298</v>
       </c>
@@ -5880,10 +5880,10 @@
       <c r="L5" s="50"/>
       <c r="M5" s="50"/>
       <c r="N5" s="50"/>
-      <c r="O5" s="57" t="s">
+      <c r="O5" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="P5" s="57"/>
+      <c r="P5" s="54"/>
       <c r="Q5" s="50" t="s">
         <v>222</v>
       </c>
@@ -5891,10 +5891,10 @@
       <c r="S5" s="50"/>
       <c r="T5" s="50"/>
       <c r="U5" s="50"/>
-      <c r="V5" s="49" t="s">
+      <c r="V5" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="W5" s="49"/>
+      <c r="W5" s="51"/>
       <c r="X5" s="50" t="s">
         <v>44</v>
       </c>
@@ -5904,10 +5904,10 @@
       <c r="AB5" s="50"/>
     </row>
     <row r="6" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="52" t="s">
         <v>346</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="50" t="s">
         <v>212</v>
       </c>
@@ -5915,10 +5915,10 @@
       <c r="E6" s="50"/>
       <c r="F6" s="50"/>
       <c r="G6" s="50"/>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="52" t="s">
         <v>299</v>
       </c>
-      <c r="I6" s="53"/>
+      <c r="I6" s="52"/>
       <c r="J6" s="50" t="s">
         <v>37</v>
       </c>
@@ -5926,10 +5926,10 @@
       <c r="L6" s="50"/>
       <c r="M6" s="50"/>
       <c r="N6" s="50"/>
-      <c r="O6" s="57" t="s">
+      <c r="O6" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="P6" s="57"/>
+      <c r="P6" s="54"/>
       <c r="Q6" s="50" t="s">
         <v>222</v>
       </c>
@@ -5937,8 +5937,8 @@
       <c r="S6" s="50"/>
       <c r="T6" s="50"/>
       <c r="U6" s="50"/>
-      <c r="V6" s="49"/>
-      <c r="W6" s="49"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="51"/>
       <c r="X6" s="50"/>
       <c r="Y6" s="50"/>
       <c r="Z6" s="50"/>
@@ -5946,10 +5946,10 @@
       <c r="AB6" s="50"/>
     </row>
     <row r="7" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="52" t="s">
         <v>445</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="50" t="s">
         <v>38</v>
       </c>
@@ -5968,10 +5968,10 @@
       <c r="L7" s="50"/>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
-      <c r="O7" s="57" t="s">
+      <c r="O7" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="P7" s="57"/>
+      <c r="P7" s="54"/>
       <c r="Q7" s="50" t="s">
         <v>223</v>
       </c>
@@ -5979,10 +5979,10 @@
       <c r="S7" s="50"/>
       <c r="T7" s="50"/>
       <c r="U7" s="50"/>
-      <c r="V7" s="49" t="s">
+      <c r="V7" s="51" t="s">
         <v>340</v>
       </c>
-      <c r="W7" s="49"/>
+      <c r="W7" s="51"/>
       <c r="X7" s="50" t="s">
         <v>45</v>
       </c>
@@ -5992,28 +5992,28 @@
       <c r="AB7" s="50"/>
     </row>
     <row r="8" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="57" t="s">
+      <c r="B8" s="52"/>
+      <c r="C8" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="50"/>
       <c r="K8" s="50"/>
       <c r="L8" s="50"/>
       <c r="M8" s="50"/>
       <c r="N8" s="50"/>
-      <c r="O8" s="57" t="s">
+      <c r="O8" s="54" t="s">
         <v>312</v>
       </c>
-      <c r="P8" s="57"/>
+      <c r="P8" s="54"/>
       <c r="Q8" s="50" t="s">
         <v>223</v>
       </c>
@@ -6021,10 +6021,10 @@
       <c r="S8" s="50"/>
       <c r="T8" s="50"/>
       <c r="U8" s="50"/>
-      <c r="V8" s="49" t="s">
+      <c r="V8" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="W8" s="49"/>
+      <c r="W8" s="51"/>
       <c r="X8" s="50" t="s">
         <v>41</v>
       </c>
@@ -6034,21 +6034,21 @@
       <c r="AB8" s="50"/>
     </row>
     <row r="9" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="52" t="s">
         <v>310</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="57" t="s">
+      <c r="B9" s="52"/>
+      <c r="C9" s="54" t="s">
         <v>211</v>
       </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="53" t="s">
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="52" t="s">
         <v>305</v>
       </c>
-      <c r="I9" s="53"/>
+      <c r="I9" s="52"/>
       <c r="J9" s="50" t="s">
         <v>308</v>
       </c>
@@ -6056,21 +6056,21 @@
       <c r="L9" s="50"/>
       <c r="M9" s="50"/>
       <c r="N9" s="50"/>
-      <c r="O9" s="57" t="s">
+      <c r="O9" s="54" t="s">
         <v>301</v>
       </c>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="57" t="s">
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54" t="s">
         <v>266</v>
       </c>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
-      <c r="U9" s="57"/>
-      <c r="V9" s="49" t="s">
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="54"/>
+      <c r="U9" s="54"/>
+      <c r="V9" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="W9" s="49"/>
+      <c r="W9" s="51"/>
       <c r="X9" s="50" t="s">
         <v>48</v>
       </c>
@@ -6080,21 +6080,21 @@
       <c r="AB9" s="50"/>
     </row>
     <row r="10" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="57" t="s">
+      <c r="B10" s="52"/>
+      <c r="C10" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="53" t="s">
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="52" t="s">
         <v>431</v>
       </c>
-      <c r="I10" s="53"/>
+      <c r="I10" s="52"/>
       <c r="J10" s="50" t="s">
         <v>432</v>
       </c>
@@ -6102,10 +6102,10 @@
       <c r="L10" s="50"/>
       <c r="M10" s="50"/>
       <c r="N10" s="50"/>
-      <c r="O10" s="49" t="s">
+      <c r="O10" s="54" t="s">
         <v>433</v>
       </c>
-      <c r="P10" s="49"/>
+      <c r="P10" s="54"/>
       <c r="Q10" s="50" t="s">
         <v>434</v>
       </c>
@@ -6113,10 +6113,10 @@
       <c r="S10" s="50"/>
       <c r="T10" s="50"/>
       <c r="U10" s="50"/>
-      <c r="V10" s="49" t="s">
+      <c r="V10" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="W10" s="49"/>
+      <c r="W10" s="51"/>
       <c r="X10" s="50" t="s">
         <v>51</v>
       </c>
@@ -6126,17 +6126,17 @@
       <c r="AB10" s="50"/>
     </row>
     <row r="11" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="61" t="s">
+      <c r="B11" s="52"/>
+      <c r="C11" s="57" t="s">
         <v>216</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="58" t="s">
         <v>304</v>
       </c>
@@ -6148,10 +6148,10 @@
       <c r="L11" s="50"/>
       <c r="M11" s="50"/>
       <c r="N11" s="50"/>
-      <c r="O11" s="49" t="s">
+      <c r="O11" s="54" t="s">
         <v>300</v>
       </c>
-      <c r="P11" s="49"/>
+      <c r="P11" s="54"/>
       <c r="Q11" s="50" t="s">
         <v>341</v>
       </c>
@@ -6159,10 +6159,10 @@
       <c r="S11" s="50"/>
       <c r="T11" s="50"/>
       <c r="U11" s="50"/>
-      <c r="V11" s="49" t="s">
+      <c r="V11" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="W11" s="49"/>
+      <c r="W11" s="51"/>
       <c r="X11" s="50" t="s">
         <v>436</v>
       </c>
@@ -6172,21 +6172,21 @@
       <c r="AB11" s="50"/>
     </row>
     <row r="12" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="52" t="s">
         <v>446</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="60" t="s">
+      <c r="B12" s="52"/>
+      <c r="C12" s="53" t="s">
         <v>219</v>
       </c>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="53" t="s">
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="52" t="s">
         <v>303</v>
       </c>
-      <c r="I12" s="53"/>
+      <c r="I12" s="52"/>
       <c r="J12" s="50" t="s">
         <v>210</v>
       </c>
@@ -6194,19 +6194,19 @@
       <c r="L12" s="50"/>
       <c r="M12" s="50"/>
       <c r="N12" s="50"/>
-      <c r="O12" s="57" t="s">
+      <c r="O12" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="P12" s="57"/>
+      <c r="P12" s="54"/>
       <c r="Q12" s="50"/>
       <c r="R12" s="50"/>
       <c r="S12" s="50"/>
       <c r="T12" s="50"/>
       <c r="U12" s="50"/>
-      <c r="V12" s="59" t="s">
+      <c r="V12" s="49" t="s">
         <v>218</v>
       </c>
-      <c r="W12" s="59"/>
+      <c r="W12" s="49"/>
       <c r="X12" s="50" t="s">
         <v>45</v>
       </c>
@@ -6216,21 +6216,21 @@
       <c r="AB12" s="50"/>
     </row>
     <row r="13" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="52" t="s">
         <v>220</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="60" t="s">
+      <c r="B13" s="52"/>
+      <c r="C13" s="53" t="s">
         <v>221</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
       <c r="G13" s="50"/>
-      <c r="H13" s="53" t="s">
+      <c r="H13" s="52" t="s">
         <v>309</v>
       </c>
-      <c r="I13" s="53"/>
+      <c r="I13" s="52"/>
       <c r="J13" s="50" t="s">
         <v>36</v>
       </c>
@@ -6238,21 +6238,21 @@
       <c r="L13" s="50"/>
       <c r="M13" s="50"/>
       <c r="N13" s="50"/>
-      <c r="O13" s="68" t="s">
+      <c r="O13" s="55" t="s">
         <v>302</v>
       </c>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="69" t="s">
+      <c r="P13" s="55"/>
+      <c r="Q13" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="R13" s="69"/>
-      <c r="S13" s="69"/>
-      <c r="T13" s="69"/>
-      <c r="U13" s="69"/>
-      <c r="V13" s="49" t="s">
+      <c r="R13" s="56"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="56"/>
+      <c r="U13" s="56"/>
+      <c r="V13" s="51" t="s">
         <v>437</v>
       </c>
-      <c r="W13" s="49"/>
+      <c r="W13" s="51"/>
       <c r="X13" s="50"/>
       <c r="Y13" s="50"/>
       <c r="Z13" s="50"/>
@@ -6260,10 +6260,10 @@
       <c r="AB13" s="50"/>
     </row>
     <row r="14" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="52" t="s">
         <v>313</v>
       </c>
-      <c r="B14" s="53"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="50" t="s">
         <v>430</v>
       </c>
@@ -6271,25 +6271,26 @@
       <c r="E14" s="50"/>
       <c r="F14" s="50"/>
       <c r="G14" s="50"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
       <c r="L14" s="50"/>
       <c r="M14" s="50"/>
       <c r="N14" s="50"/>
-      <c r="O14" s="17" t="s">
+      <c r="O14" s="58" t="s">
         <v>447</v>
       </c>
+      <c r="P14" s="58"/>
       <c r="Q14" s="50"/>
       <c r="R14" s="50"/>
       <c r="S14" s="50"/>
       <c r="T14" s="50"/>
       <c r="U14" s="50"/>
-      <c r="V14" s="49" t="s">
+      <c r="V14" s="51" t="s">
         <v>441</v>
       </c>
-      <c r="W14" s="49"/>
+      <c r="W14" s="51"/>
       <c r="X14" s="50" t="s">
         <v>440</v>
       </c>
@@ -6299,15 +6300,15 @@
       <c r="AB14" s="50"/>
     </row>
     <row r="15" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
       <c r="J15" s="50"/>
       <c r="K15" s="50"/>
       <c r="L15" s="50"/>
       <c r="M15" s="50"/>
       <c r="N15" s="50"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
       <c r="Q15" s="50"/>
       <c r="R15" s="50"/>
       <c r="S15" s="50"/>
@@ -6315,22 +6316,22 @@
       <c r="U15" s="50"/>
     </row>
     <row r="16" spans="1:30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
       <c r="J16" s="50"/>
       <c r="K16" s="50"/>
       <c r="L16" s="50"/>
       <c r="M16" s="50"/>
       <c r="N16" s="50"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="49"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
       <c r="Q16" s="50"/>
       <c r="R16" s="50"/>
       <c r="S16" s="50"/>
       <c r="T16" s="50"/>
       <c r="U16" s="50"/>
-      <c r="V16" s="49"/>
-      <c r="W16" s="49"/>
+      <c r="V16" s="51"/>
+      <c r="W16" s="51"/>
       <c r="X16" s="50"/>
       <c r="Y16" s="50"/>
       <c r="Z16" s="50"/>
@@ -6338,22 +6339,22 @@
       <c r="AB16" s="50"/>
     </row>
     <row r="17" spans="1:28" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="50"/>
       <c r="K17" s="50"/>
       <c r="L17" s="50"/>
       <c r="M17" s="50"/>
       <c r="N17" s="50"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="49"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
       <c r="Q17" s="50"/>
       <c r="R17" s="50"/>
       <c r="S17" s="50"/>
       <c r="T17" s="50"/>
       <c r="U17" s="50"/>
-      <c r="V17" s="49"/>
-      <c r="W17" s="49"/>
+      <c r="V17" s="51"/>
+      <c r="W17" s="51"/>
       <c r="X17" s="50"/>
       <c r="Y17" s="50"/>
       <c r="Z17" s="50"/>
@@ -6361,29 +6362,29 @@
       <c r="AB17" s="50"/>
     </row>
     <row r="18" spans="1:28" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="59"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="50"/>
       <c r="D18" s="50"/>
       <c r="E18" s="50"/>
       <c r="F18" s="50"/>
       <c r="G18" s="50"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
       <c r="L18" s="50"/>
       <c r="M18" s="50"/>
       <c r="N18" s="50"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
       <c r="Q18" s="50"/>
       <c r="R18" s="50"/>
       <c r="S18" s="50"/>
       <c r="T18" s="50"/>
       <c r="U18" s="50"/>
-      <c r="V18" s="49"/>
-      <c r="W18" s="49"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
       <c r="X18" s="50"/>
       <c r="Y18" s="50"/>
       <c r="Z18" s="50"/>
@@ -6391,29 +6392,29 @@
       <c r="AB18" s="50"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
-      <c r="B19" s="59"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="50"/>
       <c r="D19" s="50"/>
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
       <c r="G19" s="50"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
       <c r="J19" s="50"/>
       <c r="K19" s="50"/>
       <c r="L19" s="50"/>
       <c r="M19" s="50"/>
       <c r="N19" s="50"/>
-      <c r="O19" s="49"/>
-      <c r="P19" s="49"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
       <c r="Q19" s="50"/>
       <c r="R19" s="50"/>
       <c r="S19" s="50"/>
       <c r="T19" s="50"/>
       <c r="U19" s="50"/>
-      <c r="V19" s="49"/>
-      <c r="W19" s="49"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="51"/>
       <c r="X19" s="50"/>
       <c r="Y19" s="50"/>
       <c r="Z19" s="50"/>
@@ -6421,29 +6422,29 @@
       <c r="AB19" s="50"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
-      <c r="B20" s="59"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="50"/>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>
       <c r="F20" s="50"/>
       <c r="G20" s="50"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
       <c r="J20" s="50"/>
       <c r="K20" s="50"/>
       <c r="L20" s="50"/>
       <c r="M20" s="50"/>
       <c r="N20" s="50"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="49"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
       <c r="Q20" s="50"/>
       <c r="R20" s="50"/>
       <c r="S20" s="50"/>
       <c r="T20" s="50"/>
       <c r="U20" s="50"/>
-      <c r="V20" s="49"/>
-      <c r="W20" s="49"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
       <c r="X20" s="50"/>
       <c r="Y20" s="50"/>
       <c r="Z20" s="50"/>
@@ -6451,29 +6452,29 @@
       <c r="AB20" s="50"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
-      <c r="B21" s="59"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="50"/>
       <c r="D21" s="50"/>
       <c r="E21" s="50"/>
       <c r="F21" s="50"/>
       <c r="G21" s="50"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="59"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
       <c r="J21" s="50"/>
       <c r="K21" s="50"/>
       <c r="L21" s="50"/>
       <c r="M21" s="50"/>
       <c r="N21" s="50"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="49"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
       <c r="Q21" s="50"/>
       <c r="R21" s="50"/>
       <c r="S21" s="50"/>
       <c r="T21" s="50"/>
       <c r="U21" s="50"/>
-      <c r="V21" s="49"/>
-      <c r="W21" s="49"/>
+      <c r="V21" s="51"/>
+      <c r="W21" s="51"/>
       <c r="X21" s="50"/>
       <c r="Y21" s="50"/>
       <c r="Z21" s="50"/>
@@ -6481,29 +6482,29 @@
       <c r="AB21" s="50"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="59"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="50"/>
       <c r="D22" s="50"/>
       <c r="E22" s="50"/>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="59"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
       <c r="J22" s="50"/>
       <c r="K22" s="50"/>
       <c r="L22" s="50"/>
       <c r="M22" s="50"/>
       <c r="N22" s="50"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
+      <c r="O22" s="51"/>
+      <c r="P22" s="51"/>
       <c r="Q22" s="50"/>
       <c r="R22" s="50"/>
       <c r="S22" s="50"/>
       <c r="T22" s="50"/>
       <c r="U22" s="50"/>
-      <c r="V22" s="49"/>
-      <c r="W22" s="49"/>
+      <c r="V22" s="51"/>
+      <c r="W22" s="51"/>
       <c r="X22" s="50"/>
       <c r="Y22" s="50"/>
       <c r="Z22" s="50"/>
@@ -6511,22 +6512,22 @@
       <c r="AB22" s="50"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-      <c r="B23" s="59"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
       <c r="E23" s="50"/>
       <c r="F23" s="50"/>
       <c r="G23" s="50"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
       <c r="J23" s="50"/>
       <c r="K23" s="50"/>
       <c r="L23" s="50"/>
       <c r="M23" s="50"/>
       <c r="N23" s="50"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="49"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
       <c r="Q23" s="50"/>
       <c r="R23" s="50"/>
       <c r="S23" s="50"/>
@@ -6534,22 +6535,22 @@
       <c r="U23" s="50"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="59"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="50"/>
       <c r="D24" s="50"/>
       <c r="E24" s="50"/>
       <c r="F24" s="50"/>
       <c r="G24" s="50"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
       <c r="J24" s="50"/>
       <c r="K24" s="50"/>
       <c r="L24" s="50"/>
       <c r="M24" s="50"/>
       <c r="N24" s="50"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="49"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
       <c r="Q24" s="50"/>
       <c r="R24" s="50"/>
       <c r="S24" s="50"/>
@@ -6557,22 +6558,22 @@
       <c r="U24" s="50"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="59"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
       <c r="E25" s="50"/>
       <c r="F25" s="50"/>
       <c r="G25" s="50"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
       <c r="J25" s="50"/>
       <c r="K25" s="50"/>
       <c r="L25" s="50"/>
       <c r="M25" s="50"/>
       <c r="N25" s="50"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="49"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
       <c r="Q25" s="50"/>
       <c r="R25" s="50"/>
       <c r="S25" s="50"/>
@@ -6580,22 +6581,22 @@
       <c r="U25" s="50"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
-      <c r="B26" s="59"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="50"/>
       <c r="D26" s="50"/>
       <c r="E26" s="50"/>
       <c r="F26" s="50"/>
       <c r="G26" s="50"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
       <c r="J26" s="50"/>
       <c r="K26" s="50"/>
       <c r="L26" s="50"/>
       <c r="M26" s="50"/>
       <c r="N26" s="50"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="49"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="51"/>
       <c r="Q26" s="50"/>
       <c r="R26" s="50"/>
       <c r="S26" s="50"/>
@@ -6603,22 +6604,22 @@
       <c r="U26" s="50"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
-      <c r="B27" s="59"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
       <c r="E27" s="50"/>
       <c r="F27" s="50"/>
       <c r="G27" s="50"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
       <c r="J27" s="50"/>
       <c r="K27" s="50"/>
       <c r="L27" s="50"/>
       <c r="M27" s="50"/>
       <c r="N27" s="50"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="49"/>
+      <c r="O27" s="51"/>
+      <c r="P27" s="51"/>
       <c r="Q27" s="50"/>
       <c r="R27" s="50"/>
       <c r="S27" s="50"/>
@@ -6626,22 +6627,22 @@
       <c r="U27" s="50"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
-      <c r="B28" s="59"/>
+      <c r="A28" s="49"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="50"/>
       <c r="D28" s="50"/>
       <c r="E28" s="50"/>
       <c r="F28" s="50"/>
       <c r="G28" s="50"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
       <c r="J28" s="50"/>
       <c r="K28" s="50"/>
       <c r="L28" s="50"/>
       <c r="M28" s="50"/>
       <c r="N28" s="50"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
       <c r="Q28" s="50"/>
       <c r="R28" s="50"/>
       <c r="S28" s="50"/>
@@ -6649,22 +6650,22 @@
       <c r="U28" s="50"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
-      <c r="B29" s="59"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="50"/>
       <c r="D29" s="50"/>
       <c r="E29" s="50"/>
       <c r="F29" s="50"/>
       <c r="G29" s="50"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
       <c r="J29" s="50"/>
       <c r="K29" s="50"/>
       <c r="L29" s="50"/>
       <c r="M29" s="50"/>
       <c r="N29" s="50"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="51"/>
       <c r="Q29" s="50"/>
       <c r="R29" s="50"/>
       <c r="S29" s="50"/>
@@ -6672,22 +6673,22 @@
       <c r="U29" s="50"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="59"/>
-      <c r="B30" s="59"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="50"/>
       <c r="D30" s="50"/>
       <c r="E30" s="50"/>
       <c r="F30" s="50"/>
       <c r="G30" s="50"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="59"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
       <c r="J30" s="50"/>
       <c r="K30" s="50"/>
       <c r="L30" s="50"/>
       <c r="M30" s="50"/>
       <c r="N30" s="50"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
       <c r="Q30" s="50"/>
       <c r="R30" s="50"/>
       <c r="S30" s="50"/>
@@ -6695,22 +6696,22 @@
       <c r="U30" s="50"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="59"/>
-      <c r="B31" s="59"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="50"/>
       <c r="D31" s="50"/>
       <c r="E31" s="50"/>
       <c r="F31" s="50"/>
       <c r="G31" s="50"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
       <c r="J31" s="50"/>
       <c r="K31" s="50"/>
       <c r="L31" s="50"/>
       <c r="M31" s="50"/>
       <c r="N31" s="50"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
+      <c r="O31" s="51"/>
+      <c r="P31" s="51"/>
       <c r="Q31" s="50"/>
       <c r="R31" s="50"/>
       <c r="S31" s="50"/>
@@ -6718,22 +6719,22 @@
       <c r="U31" s="50"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
-      <c r="B32" s="59"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="50"/>
       <c r="D32" s="50"/>
       <c r="E32" s="50"/>
       <c r="F32" s="50"/>
       <c r="G32" s="50"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="59"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
       <c r="J32" s="50"/>
       <c r="K32" s="50"/>
       <c r="L32" s="50"/>
       <c r="M32" s="50"/>
       <c r="N32" s="50"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
+      <c r="O32" s="51"/>
+      <c r="P32" s="51"/>
       <c r="Q32" s="50"/>
       <c r="R32" s="50"/>
       <c r="S32" s="50"/>
@@ -6741,22 +6742,22 @@
       <c r="U32" s="50"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
-      <c r="B33" s="59"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="50"/>
       <c r="D33" s="50"/>
       <c r="E33" s="50"/>
       <c r="F33" s="50"/>
       <c r="G33" s="50"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
       <c r="J33" s="50"/>
       <c r="K33" s="50"/>
       <c r="L33" s="50"/>
       <c r="M33" s="50"/>
       <c r="N33" s="50"/>
-      <c r="O33" s="59"/>
-      <c r="P33" s="59"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
       <c r="Q33" s="50"/>
       <c r="R33" s="50"/>
       <c r="S33" s="50"/>
@@ -6764,22 +6765,22 @@
       <c r="U33" s="50"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
-      <c r="B34" s="59"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="50"/>
       <c r="D34" s="50"/>
       <c r="E34" s="50"/>
       <c r="F34" s="50"/>
       <c r="G34" s="50"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="59"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
       <c r="J34" s="50"/>
       <c r="K34" s="50"/>
       <c r="L34" s="50"/>
       <c r="M34" s="50"/>
       <c r="N34" s="50"/>
-      <c r="O34" s="59"/>
-      <c r="P34" s="59"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
       <c r="Q34" s="50"/>
       <c r="R34" s="50"/>
       <c r="S34" s="50"/>
@@ -6787,8 +6788,8 @@
       <c r="U34" s="50"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
-      <c r="B35" s="59"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="50"/>
       <c r="D35" s="50"/>
       <c r="E35" s="50"/>
@@ -6796,144 +6797,75 @@
       <c r="G35" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="229">
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:U34"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:U33"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:U32"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:U31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:U30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:U29"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:U28"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:U26"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:U25"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:U24"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:U23"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="X22:AB22"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:AB21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:U21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:U22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="X20:AB20"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="X19:AB19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:U19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:U20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:AB18"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:AB17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:U17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:U18"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="X14:AB14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:U15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:U16"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="X13:AB13"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:G14"/>
+  <mergeCells count="230">
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:AB5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:AB4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:N2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="V1:AB2"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="O1:U2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:AB7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:U10"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="X11:AB11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:U11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:N11"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="H10:I10"/>
@@ -6958,74 +6890,144 @@
     <mergeCell ref="J13:N13"/>
     <mergeCell ref="X12:AB12"/>
     <mergeCell ref="X16:AB16"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:U10"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="X11:AB11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:U11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:AB8"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:AB7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:N2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="V1:AB2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="O1:U2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:AB5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:AB4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="X14:AB14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:U16"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="X13:AB13"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="X18:AB18"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:AB17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:U17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:U18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="X20:AB20"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="X19:AB19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:U19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:U20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="X22:AB22"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:AB21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:U21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:U22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:U24"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:U23"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:U26"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:U28"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:U30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:U29"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:U32"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:U31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:U34"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:U33"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:G33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C13" r:id="rId1" xr:uid="{868F8F85-B252-4B04-B081-E9B23AD46A23}"/>
@@ -7060,13 +7062,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="66" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -7086,13 +7088,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
@@ -7235,13 +7237,13 @@
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="64" t="s">
         <v>428</v>
       </c>
-      <c r="B19" s="62"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
@@ -7293,16 +7295,16 @@
       <c r="A25" s="14" t="s">
         <v>429</v>
       </c>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
@@ -7350,15 +7352,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="68" t="s">
         <v>247</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -7370,12 +7372,12 @@
       <c r="C2" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="69" t="s">
         <v>228</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
       <c r="I2" s="20" t="s">
         <v>278</v>
       </c>
@@ -7390,12 +7392,12 @@
       <c r="C3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="67" t="s">
         <v>249</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
       <c r="I3" s="5" t="s">
         <v>279</v>
       </c>
@@ -7413,12 +7415,12 @@
       <c r="C4" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="67" t="s">
         <v>256</v>
       </c>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
       <c r="J4" s="5" t="s">
         <v>282</v>
       </c>
@@ -7433,12 +7435,12 @@
       <c r="C5" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
       <c r="J5" s="5" t="s">
         <v>283</v>
       </c>
@@ -7453,12 +7455,12 @@
       <c r="C6" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="67" t="s">
         <v>250</v>
       </c>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -7475,10 +7477,10 @@
       <c r="A10" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
       <c r="I10" s="5" t="s">
         <v>156</v>
       </c>
@@ -7496,12 +7498,12 @@
       <c r="C11" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="67" t="s">
         <v>286</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
       <c r="J11" s="5" t="s">
         <v>288</v>
       </c>
@@ -7516,12 +7518,12 @@
       <c r="C12" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D12" s="65" t="s">
+      <c r="D12" s="67" t="s">
         <v>262</v>
       </c>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
       <c r="I12" s="5" t="s">
         <v>290</v>
       </c>
@@ -7539,12 +7541,12 @@
       <c r="C13" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D13" s="65" t="s">
+      <c r="D13" s="67" t="s">
         <v>265</v>
       </c>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -7556,24 +7558,24 @@
       <c r="C14" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="D14" s="65" t="s">
+      <c r="D14" s="67" t="s">
         <v>295</v>
       </c>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
     </row>
     <row r="17" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -7585,93 +7587,108 @@
       <c r="C17" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="D20:G20"/>
@@ -7684,21 +7701,6 @@
     <mergeCell ref="D27:G27"/>
     <mergeCell ref="D28:G28"/>
     <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>